<commit_message>
Add Obsidian Flames Ultra Rares
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AE41DD-E305-40FB-9CC6-2C95C3051FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECAE10A-DBBB-4A11-90D8-F89AE34427F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7236" yWindow="780" windowWidth="12576" windowHeight="9396" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,17 +570,17 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="A2" s="8">
         <v>45149</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -593,7 +593,7 @@
       </c>
       <c r="B3" s="3">
         <f ca="1">IF(A3 = "TBA", "TBA", IF(A3 - TODAY() &gt; 0, A3 - TODAY(), "out now"))</f>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -611,7 +611,7 @@
       </c>
       <c r="B4" s="5">
         <f t="shared" ref="B4:B5" ca="1" si="1">IF(A4 = "TBA", "TBA", IF(A4 - TODAY() &gt; 0, A4 - TODAY(), "out now"))</f>
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>8</v>
@@ -629,7 +629,7 @@
       </c>
       <c r="B5" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -647,7 +647,7 @@
       </c>
       <c r="B6" s="5">
         <f t="shared" ref="B6" ca="1" si="2">IF(A6 = "TBA", "TBA", IF(A6 - TODAY() &gt; 0, A6 - TODAY(), "out now"))</f>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>27</v>
@@ -662,7 +662,7 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" ca="1" si="3">IF(A7 = "TBA", "TBA", IF(A7 - TODAY() &gt; 0, A7 - TODAY(), "out now"))</f>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
@@ -682,8 +682,8 @@
         <v>45191</v>
       </c>
       <c r="B8" s="5">
-        <f ca="1">IF(A8 = "TBA", "TBA", IF(A8 - TODAY() &gt; 0, A8 - TODAY(), "out now"))</f>
-        <v>49</v>
+        <f t="shared" ref="B8:B18" ca="1" si="4">IF(A8 = "TBA", "TBA", IF(A8 - TODAY() &gt; 0, A8 - TODAY(), "out now"))</f>
+        <v>43</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>28</v>
@@ -697,8 +697,8 @@
         <v>45191</v>
       </c>
       <c r="B9" s="5">
-        <f ca="1">IF(A9 = "TBA", "TBA", IF(A9 - TODAY() &gt; 0, A9 - TODAY(), "out now"))</f>
-        <v>49</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>43</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
@@ -712,8 +712,8 @@
         <v>45205</v>
       </c>
       <c r="B10" s="5">
-        <f ca="1">IF(A10 = "TBA", "TBA", IF(A10 - TODAY() &gt; 0, A10 - TODAY(), "out now"))</f>
-        <v>63</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>57</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>29</v>
@@ -727,8 +727,8 @@
         <v>45205</v>
       </c>
       <c r="B11" s="5">
-        <f ca="1">IF(A11 = "TBA", "TBA", IF(A11 - TODAY() &gt; 0, A11 - TODAY(), "out now"))</f>
-        <v>63</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>57</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>30</v>
@@ -742,8 +742,8 @@
         <v>45205</v>
       </c>
       <c r="B12" s="5">
-        <f ca="1">IF(A12 = "TBA", "TBA", IF(A12 - TODAY() &gt; 0, A12 - TODAY(), "out now"))</f>
-        <v>63</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>57</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>31</v>
@@ -757,8 +757,8 @@
         <v>45205</v>
       </c>
       <c r="B13" s="5">
-        <f ca="1">IF(A13 = "TBA", "TBA", IF(A13 - TODAY() &gt; 0, A13 - TODAY(), "out now"))</f>
-        <v>63</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>57</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>32</v>
@@ -772,8 +772,8 @@
         <v>45219</v>
       </c>
       <c r="B14" s="5">
-        <f ca="1">IF(A14 = "TBA", "TBA", IF(A14 - TODAY() &gt; 0, A14 - TODAY(), "out now"))</f>
-        <v>77</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>71</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>17</v>
@@ -787,8 +787,8 @@
         <v>45233</v>
       </c>
       <c r="B15" s="5">
-        <f ca="1">IF(A15 = "TBA", "TBA", IF(A15 - TODAY() &gt; 0, A15 - TODAY(), "out now"))</f>
-        <v>91</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>85</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>1</v>
@@ -802,8 +802,8 @@
         <v>45233</v>
       </c>
       <c r="B16" s="5">
-        <f ca="1">IF(A16 = "TBA", "TBA", IF(A16 - TODAY() &gt; 0, A16 - TODAY(), "out now"))</f>
-        <v>91</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>85</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>9</v>
@@ -817,7 +817,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="6" t="str">
-        <f ca="1">IF(A17 = "TBA", "TBA", IF(A17 - TODAY() &gt; 0, A17 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>TBA</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -832,7 +832,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="6" t="str">
-        <f ca="1">IF(A18 = "TBA", "TBA", IF(A18 - TODAY() &gt; 0, A18 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>TBA</v>
       </c>
       <c r="C18" s="6" t="s">

</xml_diff>

<commit_message>
Fix bugs, add extremely rare cards page
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E766D6D-DD82-44A8-AE01-DF382F4685EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFF0035-AAF7-4A08-B96C-4EF4E0A01968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6336" yWindow="2064" windowWidth="12576" windowHeight="9396" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -542,7 +542,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,17 +610,17 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
-        <v>45169</v>
+        <v>45167</v>
       </c>
       <c r="B4" s="5">
-        <f t="shared" ref="B4:B5" ca="1" si="1">IF(A4 = "TBA", "TBA", IF(A4 - TODAY() &gt; 0, A4 - TODAY(), "out now"))</f>
-        <v>12</v>
+        <f ca="1">IF(A4 = "TBA", "TBA", IF(A4 - TODAY() &gt; 0, A4 - TODAY(), "out now"))</f>
+        <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>23</v>
@@ -631,8 +631,8 @@
         <v>45170</v>
       </c>
       <c r="B5" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <f ca="1">IF(A5 = "TBA", "TBA", IF(A5 - TODAY() &gt; 0, A5 - TODAY(), "out now"))</f>
+        <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -649,8 +649,8 @@
         <v>45170</v>
       </c>
       <c r="B6" s="5">
-        <f t="shared" ref="B6" ca="1" si="2">IF(A6 = "TBA", "TBA", IF(A6 - TODAY() &gt; 0, A6 - TODAY(), "out now"))</f>
-        <v>13</v>
+        <f t="shared" ref="B6" ca="1" si="1">IF(A6 = "TBA", "TBA", IF(A6 - TODAY() &gt; 0, A6 - TODAY(), "out now"))</f>
+        <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>27</v>
@@ -664,8 +664,8 @@
         <v>45170</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" ref="B7" ca="1" si="3">IF(A7 = "TBA", "TBA", IF(A7 - TODAY() &gt; 0, A7 - TODAY(), "out now"))</f>
-        <v>13</v>
+        <f t="shared" ref="B7" ca="1" si="2">IF(A7 = "TBA", "TBA", IF(A7 - TODAY() &gt; 0, A7 - TODAY(), "out now"))</f>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
@@ -685,8 +685,8 @@
         <v>45191</v>
       </c>
       <c r="B8" s="5">
-        <f t="shared" ref="B8:B18" ca="1" si="4">IF(A8 = "TBA", "TBA", IF(A8 - TODAY() &gt; 0, A8 - TODAY(), "out now"))</f>
-        <v>34</v>
+        <f ca="1">IF(A8 = "TBA", "TBA", IF(A8 - TODAY() &gt; 0, A8 - TODAY(), "out now"))</f>
+        <v>32</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>28</v>
@@ -700,8 +700,8 @@
         <v>45191</v>
       </c>
       <c r="B9" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>34</v>
+        <f ca="1">IF(A9 = "TBA", "TBA", IF(A9 - TODAY() &gt; 0, A9 - TODAY(), "out now"))</f>
+        <v>32</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
@@ -715,8 +715,8 @@
         <v>45205</v>
       </c>
       <c r="B10" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>48</v>
+        <f ca="1">IF(A10 = "TBA", "TBA", IF(A10 - TODAY() &gt; 0, A10 - TODAY(), "out now"))</f>
+        <v>46</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>29</v>
@@ -730,8 +730,8 @@
         <v>45205</v>
       </c>
       <c r="B11" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>48</v>
+        <f ca="1">IF(A11 = "TBA", "TBA", IF(A11 - TODAY() &gt; 0, A11 - TODAY(), "out now"))</f>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>30</v>
@@ -745,8 +745,8 @@
         <v>45205</v>
       </c>
       <c r="B12" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>48</v>
+        <f ca="1">IF(A12 = "TBA", "TBA", IF(A12 - TODAY() &gt; 0, A12 - TODAY(), "out now"))</f>
+        <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>31</v>
@@ -760,8 +760,8 @@
         <v>45205</v>
       </c>
       <c r="B13" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>48</v>
+        <f ca="1">IF(A13 = "TBA", "TBA", IF(A13 - TODAY() &gt; 0, A13 - TODAY(), "out now"))</f>
+        <v>46</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>32</v>
@@ -775,8 +775,8 @@
         <v>45219</v>
       </c>
       <c r="B14" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>62</v>
+        <f ca="1">IF(A14 = "TBA", "TBA", IF(A14 - TODAY() &gt; 0, A14 - TODAY(), "out now"))</f>
+        <v>60</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>17</v>
@@ -790,8 +790,8 @@
         <v>45233</v>
       </c>
       <c r="B15" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>76</v>
+        <f ca="1">IF(A15 = "TBA", "TBA", IF(A15 - TODAY() &gt; 0, A15 - TODAY(), "out now"))</f>
+        <v>74</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>1</v>
@@ -805,8 +805,8 @@
         <v>45233</v>
       </c>
       <c r="B16" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>76</v>
+        <f ca="1">IF(A16 = "TBA", "TBA", IF(A16 - TODAY() &gt; 0, A16 - TODAY(), "out now"))</f>
+        <v>74</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>9</v>
@@ -816,18 +816,18 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="6" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>TBA</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>16</v>
+      <c r="A17" s="7">
+        <v>45291</v>
+      </c>
+      <c r="B17" s="5">
+        <f ca="1">IF(A17 = "TBA", "TBA", IF(A17 - TODAY() &gt; 0, A17 - TODAY(), "out now"))</f>
+        <v>132</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -835,11 +835,11 @@
         <v>3</v>
       </c>
       <c r="B18" s="6" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="B18" ca="1" si="3">IF(A18 = "TBA", "TBA", IF(A18 - TODAY() &gt; 0, A18 - TODAY(), "out now"))</f>
         <v>TBA</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Add some cards and a new page
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFF0035-AAF7-4A08-B96C-4EF4E0A01968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58949BD5-3B93-4CAB-98DB-D786832613EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6336" yWindow="2064" windowWidth="12576" windowHeight="9396" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>set (ultra rares have been added)</t>
+  </si>
+  <si>
+    <t>Gyarados ex Premium Collection</t>
+  </si>
+  <si>
+    <t>check type of reverse Magikarp</t>
   </si>
 </sst>
 </file>
@@ -539,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,17 +615,17 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
-        <v>45167</v>
-      </c>
-      <c r="B4" s="5">
+      <c r="A4" s="9">
+        <v>45168</v>
+      </c>
+      <c r="B4" s="2">
         <f ca="1">IF(A4 = "TBA", "TBA", IF(A4 - TODAY() &gt; 0, A4 - TODAY(), "out now"))</f>
-        <v>8</v>
-      </c>
-      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -632,7 +638,7 @@
       </c>
       <c r="B5" s="5">
         <f ca="1">IF(A5 = "TBA", "TBA", IF(A5 - TODAY() &gt; 0, A5 - TODAY(), "out now"))</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -650,7 +656,7 @@
       </c>
       <c r="B6" s="5">
         <f t="shared" ref="B6" ca="1" si="1">IF(A6 = "TBA", "TBA", IF(A6 - TODAY() &gt; 0, A6 - TODAY(), "out now"))</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>27</v>
@@ -665,7 +671,7 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" ca="1" si="2">IF(A7 = "TBA", "TBA", IF(A7 - TODAY() &gt; 0, A7 - TODAY(), "out now"))</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
@@ -685,8 +691,8 @@
         <v>45191</v>
       </c>
       <c r="B8" s="5">
-        <f ca="1">IF(A8 = "TBA", "TBA", IF(A8 - TODAY() &gt; 0, A8 - TODAY(), "out now"))</f>
-        <v>32</v>
+        <f t="shared" ref="B8:B19" ca="1" si="3">IF(A8 = "TBA", "TBA", IF(A8 - TODAY() &gt; 0, A8 - TODAY(), "out now"))</f>
+        <v>26</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>28</v>
@@ -700,8 +706,8 @@
         <v>45191</v>
       </c>
       <c r="B9" s="5">
-        <f ca="1">IF(A9 = "TBA", "TBA", IF(A9 - TODAY() &gt; 0, A9 - TODAY(), "out now"))</f>
-        <v>32</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>26</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
@@ -715,8 +721,8 @@
         <v>45205</v>
       </c>
       <c r="B10" s="5">
-        <f ca="1">IF(A10 = "TBA", "TBA", IF(A10 - TODAY() &gt; 0, A10 - TODAY(), "out now"))</f>
-        <v>46</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>40</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>29</v>
@@ -730,8 +736,8 @@
         <v>45205</v>
       </c>
       <c r="B11" s="5">
-        <f ca="1">IF(A11 = "TBA", "TBA", IF(A11 - TODAY() &gt; 0, A11 - TODAY(), "out now"))</f>
-        <v>46</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>40</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>30</v>
@@ -745,8 +751,8 @@
         <v>45205</v>
       </c>
       <c r="B12" s="5">
-        <f ca="1">IF(A12 = "TBA", "TBA", IF(A12 - TODAY() &gt; 0, A12 - TODAY(), "out now"))</f>
-        <v>46</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>40</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>31</v>
@@ -760,8 +766,8 @@
         <v>45205</v>
       </c>
       <c r="B13" s="5">
-        <f ca="1">IF(A13 = "TBA", "TBA", IF(A13 - TODAY() &gt; 0, A13 - TODAY(), "out now"))</f>
-        <v>46</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>40</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>32</v>
@@ -775,8 +781,8 @@
         <v>45219</v>
       </c>
       <c r="B14" s="5">
-        <f ca="1">IF(A14 = "TBA", "TBA", IF(A14 - TODAY() &gt; 0, A14 - TODAY(), "out now"))</f>
-        <v>60</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>54</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>17</v>
@@ -790,8 +796,8 @@
         <v>45233</v>
       </c>
       <c r="B15" s="5">
-        <f ca="1">IF(A15 = "TBA", "TBA", IF(A15 - TODAY() &gt; 0, A15 - TODAY(), "out now"))</f>
-        <v>74</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>68</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>1</v>
@@ -805,8 +811,8 @@
         <v>45233</v>
       </c>
       <c r="B16" s="5">
-        <f ca="1">IF(A16 = "TBA", "TBA", IF(A16 - TODAY() &gt; 0, A16 - TODAY(), "out now"))</f>
-        <v>74</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>68</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>9</v>
@@ -817,31 +823,46 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
-        <v>45291</v>
+        <v>45233</v>
       </c>
       <c r="B17" s="5">
         <f ca="1">IF(A17 = "TBA", "TBA", IF(A17 - TODAY() &gt; 0, A17 - TODAY(), "out now"))</f>
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>45291</v>
+      </c>
+      <c r="B18" s="5">
+        <f ca="1">IF(A18 = "TBA", "TBA", IF(A18 - TODAY() &gt; 0, A18 - TODAY(), "out now"))</f>
+        <v>126</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="6" t="str">
-        <f t="shared" ref="B18" ca="1" si="3">IF(A18 = "TBA", "TBA", IF(A18 - TODAY() &gt; 0, A18 - TODAY(), "out now"))</f>
+      <c r="B19" s="6" t="str">
+        <f t="shared" ref="B19" ca="1" si="4">IF(A19 = "TBA", "TBA", IF(A19 - TODAY() &gt; 0, A19 - TODAY(), "out now"))</f>
         <v>TBA</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add SV 151 Ultra Rares, more future cards
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A1FA6B-A92B-435B-947E-DFE65B758838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9521B79-8C63-4D84-98C4-D9465B8DF0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7032" yWindow="2760" windowWidth="12576" windowHeight="9396" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Pokémon TCG Classic</t>
   </si>
   <si>
-    <t>TBA</t>
-  </si>
-  <si>
     <t>Pokemon TCG Collector Chest (2023)</t>
   </si>
   <si>
@@ -144,6 +141,12 @@
   </si>
   <si>
     <t>Iron Valiant ex Box</t>
+  </si>
+  <si>
+    <t>special set</t>
+  </si>
+  <si>
+    <t>SV 151</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -229,6 +232,7 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -544,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,13 +572,13 @@
         <v>out now</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -589,10 +593,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -604,13 +608,13 @@
         <v>out now</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -622,31 +626,31 @@
         <v>out now</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
-        <v>45170</v>
+        <v>45169</v>
       </c>
       <c r="B5" s="2" t="str">
         <f ca="1">IF(A5 = "TBA", "TBA", IF(A5 - TODAY() &gt; 0, A5 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -654,14 +658,14 @@
         <v>45170</v>
       </c>
       <c r="B6" s="2" t="str">
-        <f t="shared" ref="B6" ca="1" si="1">IF(A6 = "TBA", "TBA", IF(A6 - TODAY() &gt; 0, A6 - TODAY(), "out now"))</f>
+        <f ca="1">IF(A6 = "TBA", "TBA", IF(A6 - TODAY() &gt; 0, A6 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -669,80 +673,80 @@
         <v>45170</v>
       </c>
       <c r="B7" s="2" t="str">
-        <f t="shared" ref="B7" ca="1" si="2">IF(A7 = "TBA", "TBA", IF(A7 - TODAY() &gt; 0, A7 - TODAY(), "out now"))</f>
+        <f t="shared" ref="B7" ca="1" si="1">IF(A7 = "TBA", "TBA", IF(A7 - TODAY() &gt; 0, A7 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>45170</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f t="shared" ref="B8" ca="1" si="2">IF(A8 = "TBA", "TBA", IF(A8 - TODAY() &gt; 0, A8 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
         <v>45191</v>
       </c>
-      <c r="B8" s="5">
-        <f t="shared" ref="B8:B16" ca="1" si="3">IF(A8 = "TBA", "TBA", IF(A8 - TODAY() &gt; 0, A8 - TODAY(), "out now"))</f>
-        <v>20</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="B9" s="2" t="str">
+        <f t="shared" ref="B9:B18" ca="1" si="3">IF(A9 = "TBA", "TBA", IF(A9 - TODAY() &gt; 0, A9 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
         <v>45191</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B10" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <v>45205</v>
-      </c>
-      <c r="B10" s="5">
+        <v>out now</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>45191</v>
+      </c>
+      <c r="B11" s="4" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <v>45205</v>
-      </c>
-      <c r="B11" s="5">
-        <f t="shared" ca="1" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>13</v>
+        <v>out now</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -751,13 +755,13 @@
       </c>
       <c r="B12" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -766,58 +770,58 @@
       </c>
       <c r="B13" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
-        <v>45219</v>
+        <v>45205</v>
       </c>
       <c r="B14" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
-        <v>45233</v>
+        <v>45205</v>
       </c>
       <c r="B15" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
-        <v>45233</v>
+        <v>45219</v>
       </c>
       <c r="B16" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -825,74 +829,89 @@
         <v>45233</v>
       </c>
       <c r="B17" s="5">
-        <f ca="1">IF(A17 = "TBA", "TBA", IF(A17 - TODAY() &gt; 0, A17 - TODAY(), "out now"))</f>
-        <v>62</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>42</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
-        <v>45247</v>
+        <v>45233</v>
       </c>
       <c r="B18" s="5">
-        <f ca="1">IF(A18 = "TBA", "TBA", IF(A18 - TODAY() &gt; 0, A18 - TODAY(), "out now"))</f>
-        <v>76</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>42</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
-        <v>45247</v>
+        <v>45233</v>
       </c>
       <c r="B19" s="5">
         <f ca="1">IF(A19 = "TBA", "TBA", IF(A19 - TODAY() &gt; 0, A19 - TODAY(), "out now"))</f>
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
-        <v>45291</v>
+        <v>45247</v>
       </c>
       <c r="B20" s="5">
         <f ca="1">IF(A20 = "TBA", "TBA", IF(A20 - TODAY() &gt; 0, A20 - TODAY(), "out now"))</f>
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="6" t="str">
-        <f t="shared" ref="B21" ca="1" si="4">IF(A21 = "TBA", "TBA", IF(A21 - TODAY() &gt; 0, A21 - TODAY(), "out now"))</f>
-        <v>TBA</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="A21" s="7">
+        <v>45247</v>
+      </c>
+      <c r="B21" s="5">
+        <f ca="1">IF(A21 = "TBA", "TBA", IF(A21 - TODAY() &gt; 0, A21 - TODAY(), "out now"))</f>
+        <v>56</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>45247</v>
+      </c>
+      <c r="B22" s="5">
+        <f t="shared" ref="B22" ca="1" si="4">IF(A22 = "TBA", "TBA", IF(A22 - TODAY() &gt; 0, A22 - TODAY(), "out now"))</f>
+        <v>56</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>15</v>
+      <c r="D22" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add SV 151 promos
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9521B79-8C63-4D84-98C4-D9465B8DF0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFC95D9-8D5A-47F5-ACE0-E1928A65F7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="9108" yWindow="1644" windowWidth="12516" windowHeight="9396" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,17 +705,17 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="10">
         <v>45191</v>
       </c>
-      <c r="B9" s="2" t="str">
+      <c r="B9" s="4" t="str">
         <f t="shared" ref="B9:B18" ca="1" si="3">IF(A9 = "TBA", "TBA", IF(A9 - TODAY() &gt; 0, A9 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -735,17 +735,17 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="A11" s="8">
         <v>45191</v>
       </c>
-      <c r="B11" s="4" t="str">
+      <c r="B11" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>out now</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -755,7 +755,7 @@
       </c>
       <c r="B12" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>27</v>
@@ -770,7 +770,7 @@
       </c>
       <c r="B13" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>28</v>
@@ -785,7 +785,7 @@
       </c>
       <c r="B14" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>29</v>
@@ -800,7 +800,7 @@
       </c>
       <c r="B15" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>30</v>
@@ -815,7 +815,7 @@
       </c>
       <c r="B16" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>15</v>
@@ -830,7 +830,7 @@
       </c>
       <c r="B17" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>1</v>
@@ -845,7 +845,7 @@
       </c>
       <c r="B18" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>8</v>
@@ -860,7 +860,7 @@
       </c>
       <c r="B19" s="5">
         <f ca="1">IF(A19 = "TBA", "TBA", IF(A19 - TODAY() &gt; 0, A19 - TODAY(), "out now"))</f>
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>31</v>
@@ -875,7 +875,7 @@
       </c>
       <c r="B20" s="5">
         <f ca="1">IF(A20 = "TBA", "TBA", IF(A20 - TODAY() &gt; 0, A20 - TODAY(), "out now"))</f>
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>33</v>
@@ -890,7 +890,7 @@
       </c>
       <c r="B21" s="5">
         <f ca="1">IF(A21 = "TBA", "TBA", IF(A21 - TODAY() &gt; 0, A21 - TODAY(), "out now"))</f>
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>34</v>
@@ -905,7 +905,7 @@
       </c>
       <c r="B22" s="5">
         <f t="shared" ref="B22" ca="1" si="4">IF(A22 = "TBA", "TBA", IF(A22 - TODAY() &gt; 0, A22 - TODAY(), "out now"))</f>
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Add SV 151 holos
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFC95D9-8D5A-47F5-ACE0-E1928A65F7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8538D65D-3C72-441E-9947-92EEAD337D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9108" yWindow="1644" windowWidth="12516" windowHeight="9396" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
@@ -221,7 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -232,7 +232,6 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -548,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,11 +558,11 @@
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="73.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="8">
         <v>45142</v>
       </c>
@@ -577,11 +576,11 @@
       <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>45149</v>
       </c>
@@ -595,11 +594,11 @@
       <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>45156</v>
       </c>
@@ -613,11 +612,11 @@
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>45168</v>
       </c>
@@ -631,11 +630,11 @@
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>45169</v>
       </c>
@@ -649,11 +648,11 @@
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>45170</v>
       </c>
@@ -668,7 +667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>45170</v>
       </c>
@@ -682,14 +681,14 @@
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>45170</v>
       </c>
@@ -704,22 +703,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
         <v>45191</v>
       </c>
-      <c r="B9" s="4" t="str">
+      <c r="B9" s="2" t="str">
         <f t="shared" ref="B9:B18" ca="1" si="3">IF(A9 = "TBA", "TBA", IF(A9 - TODAY() &gt; 0, A9 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>45191</v>
       </c>
@@ -734,7 +733,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>45191</v>
       </c>
@@ -749,13 +748,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>45205</v>
       </c>
       <c r="B12" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>27</v>
@@ -764,13 +763,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>45205</v>
       </c>
       <c r="B13" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>28</v>
@@ -779,13 +778,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>45205</v>
       </c>
       <c r="B14" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>29</v>
@@ -794,13 +793,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>45205</v>
       </c>
       <c r="B15" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>30</v>
@@ -809,13 +808,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>45219</v>
       </c>
       <c r="B16" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>15</v>
@@ -830,7 +829,7 @@
       </c>
       <c r="B17" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>1</v>
@@ -845,7 +844,7 @@
       </c>
       <c r="B18" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>8</v>
@@ -860,7 +859,7 @@
       </c>
       <c r="B19" s="5">
         <f ca="1">IF(A19 = "TBA", "TBA", IF(A19 - TODAY() &gt; 0, A19 - TODAY(), "out now"))</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>31</v>
@@ -875,7 +874,7 @@
       </c>
       <c r="B20" s="5">
         <f ca="1">IF(A20 = "TBA", "TBA", IF(A20 - TODAY() &gt; 0, A20 - TODAY(), "out now"))</f>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>33</v>
@@ -890,7 +889,7 @@
       </c>
       <c r="B21" s="5">
         <f ca="1">IF(A21 = "TBA", "TBA", IF(A21 - TODAY() &gt; 0, A21 - TODAY(), "out now"))</f>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>34</v>
@@ -905,7 +904,7 @@
       </c>
       <c r="B22" s="5">
         <f t="shared" ref="B22" ca="1" si="4">IF(A22 = "TBA", "TBA", IF(A22 - TODAY() &gt; 0, A22 - TODAY(), "out now"))</f>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>2</v>
@@ -916,7 +915,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1" xr:uid="{2FAA5C39-4923-429D-9B10-C88CDB658962}"/>
+    <hyperlink ref="H7" r:id="rId1" xr:uid="{2FAA5C39-4923-429D-9B10-C88CDB658962}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
Add Prize Packs page
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A48DE2E-2C05-41D7-BAD3-F1BB5615D96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4C0327-6605-4523-8CA9-D8E90FADE520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10248" yWindow="1548" windowWidth="12516" windowHeight="9396" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -149,25 +149,16 @@
     <t>SV 151</t>
   </si>
   <si>
-    <t>cosmos holo Electabuzz</t>
-  </si>
-  <si>
-    <t>zapdos ex is added</t>
-  </si>
-  <si>
-    <t>alakazam ex is added</t>
-  </si>
-  <si>
     <t>Jirachi V Box</t>
   </si>
   <si>
-    <t>replace Japanese Jirachi V</t>
-  </si>
-  <si>
-    <t>check holo of Absol</t>
-  </si>
-  <si>
-    <t>cosmos holo of Abra and Kadabra</t>
+    <t>keep checking for smooth Kadabra</t>
+  </si>
+  <si>
+    <t>keep checking for smooth Absol</t>
+  </si>
+  <si>
+    <t>holos are mirage</t>
   </si>
 </sst>
 </file>
@@ -242,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -253,6 +244,7 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -570,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,75 +762,63 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
+      <c r="A12" s="8">
         <v>45191</v>
       </c>
-      <c r="B12" s="5" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>out now</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="B12" s="2" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>out now</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+      <c r="A13" s="8">
         <v>45205</v>
       </c>
-      <c r="B13" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="2" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>out now</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E13" t="s">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>45205</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>out now</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
         <v>38</v>
-      </c>
-      <c r="F13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <v>45205</v>
-      </c>
-      <c r="B14" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>45205</v>
       </c>
-      <c r="B15" s="2">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+      <c r="B15" s="2" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>out now</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>29</v>
@@ -848,42 +828,45 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
+      <c r="A16" s="10">
         <v>45205</v>
       </c>
-      <c r="B16" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>out now</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
         <v>45219</v>
       </c>
-      <c r="B17" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>17</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>out now</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>45233</v>
       </c>
       <c r="B18" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>1</v>
@@ -892,13 +875,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>45233</v>
       </c>
       <c r="B19" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>8</v>
@@ -907,13 +890,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>45233</v>
       </c>
       <c r="B20" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>31</v>
@@ -922,13 +905,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>45247</v>
       </c>
       <c r="B21" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>33</v>
@@ -937,13 +920,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>45247</v>
       </c>
       <c r="B22" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>34</v>
@@ -952,13 +935,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>45247</v>
       </c>
       <c r="B23" s="5">
         <f t="shared" ref="B23" ca="1" si="5">IF(A23 = "TBA", "TBA", IF(A23 - TODAY() &gt; 0, A23 - TODAY(), "out now"))</f>
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Add SV Promo ultra rares
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4C0327-6605-4523-8CA9-D8E90FADE520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCDA9B8-B1D1-4C3C-AF8E-1A70C8F2CAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10248" yWindow="1548" windowWidth="12516" windowHeight="9396" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>holos are mirage</t>
+  </si>
+  <si>
+    <t>ultra rares added</t>
+  </si>
+  <si>
+    <t>cosmos Lechonk</t>
   </si>
 </sst>
 </file>
@@ -562,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -828,80 +834,86 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="A16" s="8">
         <v>45205</v>
       </c>
-      <c r="B16" s="4" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>out now</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="2" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>out now</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="A17" s="8">
         <v>45219</v>
       </c>
-      <c r="B17" s="4" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>out now</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="2" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>out now</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>12</v>
+      <c r="D17" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="E17" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
+      <c r="A18" s="10">
         <v>45233</v>
       </c>
-      <c r="B18" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>out now</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
+      <c r="A19" s="10">
         <v>45233</v>
       </c>
-      <c r="B19" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>out now</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>12</v>
+      <c r="D19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
+      <c r="A20" s="9">
         <v>45233</v>
       </c>
-      <c r="B20" s="5">
-        <f t="shared" ca="1" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>out now</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -911,7 +923,7 @@
       </c>
       <c r="B21" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>33</v>
@@ -926,7 +938,7 @@
       </c>
       <c r="B22" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>34</v>
@@ -941,7 +953,7 @@
       </c>
       <c r="B23" s="5">
         <f t="shared" ref="B23" ca="1" si="5">IF(A23 = "TBA", "TBA", IF(A23 - TODAY() &gt; 0, A23 - TODAY(), "out now"))</f>
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Add Prize Pack Series 4
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B3A8F0-E56E-46DA-9912-D81B9819B285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCCBBF9-7BE3-4B42-87A9-0322FEA56313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="9876" yWindow="864" windowWidth="12516" windowHeight="9396" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="103">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -162,9 +162,6 @@
     <t>holos are mirage</t>
   </si>
   <si>
-    <t>cosmos Lechonk</t>
-  </si>
-  <si>
     <t>Wild Force &amp; Cyber Judge</t>
   </si>
   <si>
@@ -301,6 +298,54 @@
   </si>
   <si>
     <t>ultra rares added, also check blister promos</t>
+  </si>
+  <si>
+    <t>Paldea Friends Mini Tin 5-Pack</t>
+  </si>
+  <si>
+    <t>cosmos Lechonk (pixel only?)</t>
+  </si>
+  <si>
+    <t>cosmos (pixel only?)</t>
+  </si>
+  <si>
+    <t>ultra rares added</t>
+  </si>
+  <si>
+    <t>Scarlet &amp; Violet Knock Out Collection</t>
+  </si>
+  <si>
+    <t>Paldean Fates</t>
+  </si>
+  <si>
+    <t>Mabosstiff ex Box</t>
+  </si>
+  <si>
+    <t>Houndoom &amp; Melmetal ex Battle Decks</t>
+  </si>
+  <si>
+    <t>Combined Powers Premium Collection</t>
+  </si>
+  <si>
+    <t>check holo</t>
+  </si>
+  <si>
+    <t>some cards from Pokémon TCG Classic</t>
+  </si>
+  <si>
+    <t>2023 World Championships Decks</t>
+  </si>
+  <si>
+    <t>worlds cards</t>
+  </si>
+  <si>
+    <t>Paldea Adventure Chest</t>
+  </si>
+  <si>
+    <t>Temporal Forces</t>
+  </si>
+  <si>
+    <t>Iono Premium Tournament Collection</t>
   </si>
 </sst>
 </file>
@@ -407,9 +452,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -447,7 +492,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -553,7 +598,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -695,7 +740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -703,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,25 +1063,25 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="A19" s="7">
         <v>45233</v>
       </c>
-      <c r="B19" s="4" t="str">
+      <c r="B19" s="5" t="str">
         <f ca="1">IF(A19 = "TBA", "TBA", IF(A19 - TODAY() &gt; 0, A19 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1055,18 +1100,21 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
-        <v>45247</v>
-      </c>
-      <c r="B21" s="2" t="str">
+      <c r="A21" s="7">
+        <v>45233</v>
+      </c>
+      <c r="B21" s="5" t="str">
         <f ca="1">IF(A21 = "TBA", "TBA", IF(A21 - TODAY() &gt; 0, A21 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>12</v>
+      <c r="C21" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1078,25 +1126,25 @@
         <v>out now</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
+      <c r="A23" s="8">
         <v>45247</v>
       </c>
-      <c r="B23" s="5" t="str">
+      <c r="B23" s="2" t="str">
         <f ca="1">IF(A23 = "TBA", "TBA", IF(A23 - TODAY() &gt; 0, A23 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>11</v>
+      <c r="C23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1104,14 +1152,179 @@
         <v>45247</v>
       </c>
       <c r="B24" s="5" t="str">
-        <f t="shared" ref="B24" ca="1" si="5">IF(A24 = "TBA", "TBA", IF(A24 - TODAY() &gt; 0, A24 - TODAY(), "out now"))</f>
+        <f ca="1">IF(A24 = "TBA", "TBA", IF(A24 - TODAY() &gt; 0, A24 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>45247</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <f t="shared" ref="B25" ca="1" si="5">IF(A25 = "TBA", "TBA", IF(A25 - TODAY() &gt; 0, A25 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>45296</v>
+      </c>
+      <c r="B26" s="5" t="str">
+        <f ca="1">IF(A26 = "TBA", "TBA", IF(A26 - TODAY() &gt; 0, A26 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>45317</v>
+      </c>
+      <c r="B27" s="5" t="str">
+        <f ca="1">IF(A27 = "TBA", "TBA", IF(A27 - TODAY() &gt; 0, A27 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>45345</v>
+      </c>
+      <c r="B28" s="5">
+        <f ca="1">IF(A28 = "TBA", "TBA", IF(A28 - TODAY() &gt; 0, A28 - TODAY(), "out now"))</f>
+        <v>4</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>45345</v>
+      </c>
+      <c r="B29" s="5">
+        <f ca="1">IF(A29 = "TBA", "TBA", IF(A29 - TODAY() &gt; 0, A29 - TODAY(), "out now"))</f>
+        <v>4</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>45345</v>
+      </c>
+      <c r="B30" s="5">
+        <f ca="1">IF(A30 = "TBA", "TBA", IF(A30 - TODAY() &gt; 0, A30 - TODAY(), "out now"))</f>
+        <v>4</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>45352</v>
+      </c>
+      <c r="B31" s="5">
+        <f ca="1">IF(A31 = "TBA", "TBA", IF(A31 - TODAY() &gt; 0, A31 - TODAY(), "out now"))</f>
+        <v>11</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>45352</v>
+      </c>
+      <c r="B32" s="5">
+        <f ca="1">IF(A32 = "TBA", "TBA", IF(A32 - TODAY() &gt; 0, A32 - TODAY(), "out now"))</f>
+        <v>11</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>45373</v>
+      </c>
+      <c r="B33" s="5">
+        <f ca="1">IF(A33 = "TBA", "TBA", IF(A33 - TODAY() &gt; 0, A33 - TODAY(), "out now"))</f>
+        <v>32</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>45387</v>
+      </c>
+      <c r="B34" s="5">
+        <f ca="1">IF(A34 = "TBA", "TBA", IF(A34 - TODAY() &gt; 0, A34 - TODAY(), "out now"))</f>
+        <v>46</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1148,13 +1361,13 @@
         <v>out now</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1166,13 +1379,13 @@
         <v>out now</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1184,13 +1397,13 @@
         <v>out now</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1202,13 +1415,13 @@
         <v>out now</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1220,13 +1433,13 @@
         <v>out now</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1238,13 +1451,13 @@
         <v>out now</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1256,13 +1469,13 @@
         <v>out now</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1274,13 +1487,13 @@
         <v>out now</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1292,13 +1505,13 @@
         <v>out now</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1310,13 +1523,13 @@
         <v>out now</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1328,13 +1541,13 @@
         <v>out now</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1346,13 +1559,13 @@
         <v>out now</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1364,13 +1577,13 @@
         <v>out now</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1382,49 +1595,49 @@
         <v>out now</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>45317</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>out now</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>45317</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>out now</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1433,16 +1646,16 @@
       </c>
       <c r="B17" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1451,34 +1664,34 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="5"/>
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>TBA</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add some Japanese & Chinese promos
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCCBBF9-7BE3-4B42-87A9-0322FEA56313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894AFF34-E14B-4CEA-B5A2-CAC84A90D245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9876" yWindow="864" windowWidth="12516" windowHeight="9396" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="102">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -307,9 +307,6 @@
   </si>
   <si>
     <t>cosmos (pixel only?)</t>
-  </si>
-  <si>
-    <t>ultra rares added</t>
   </si>
   <si>
     <t>Scarlet &amp; Violet Knock Out Collection</t>
@@ -750,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1071,7 +1068,7 @@
         <v>45233</v>
       </c>
       <c r="B19" s="5" t="str">
-        <f ca="1">IF(A19 = "TBA", "TBA", IF(A19 - TODAY() &gt; 0, A19 - TODAY(), "out now"))</f>
+        <f t="shared" ref="B19:B24" ca="1" si="5">IF(A19 = "TBA", "TBA", IF(A19 - TODAY() &gt; 0, A19 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -1089,7 +1086,7 @@
         <v>45233</v>
       </c>
       <c r="B20" s="3" t="str">
-        <f ca="1">IF(A20 = "TBA", "TBA", IF(A20 - TODAY() &gt; 0, A20 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>out now</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1104,7 +1101,7 @@
         <v>45233</v>
       </c>
       <c r="B21" s="5" t="str">
-        <f ca="1">IF(A21 = "TBA", "TBA", IF(A21 - TODAY() &gt; 0, A21 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>out now</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -1122,7 +1119,7 @@
         <v>45247</v>
       </c>
       <c r="B22" s="2" t="str">
-        <f ca="1">IF(A22 = "TBA", "TBA", IF(A22 - TODAY() &gt; 0, A22 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>out now</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1137,7 +1134,7 @@
         <v>45247</v>
       </c>
       <c r="B23" s="2" t="str">
-        <f ca="1">IF(A23 = "TBA", "TBA", IF(A23 - TODAY() &gt; 0, A23 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>out now</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1152,7 +1149,7 @@
         <v>45247</v>
       </c>
       <c r="B24" s="5" t="str">
-        <f ca="1">IF(A24 = "TBA", "TBA", IF(A24 - TODAY() &gt; 0, A24 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>out now</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -1166,21 +1163,18 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
+      <c r="A25" s="8">
         <v>45247</v>
       </c>
-      <c r="B25" s="5" t="str">
-        <f t="shared" ref="B25" ca="1" si="5">IF(A25 = "TBA", "TBA", IF(A25 - TODAY() &gt; 0, A25 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="B25" s="2" t="str">
+        <f t="shared" ref="B25" ca="1" si="6">IF(A25 = "TBA", "TBA", IF(A25 - TODAY() &gt; 0, A25 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E25" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1188,11 +1182,11 @@
         <v>45296</v>
       </c>
       <c r="B26" s="5" t="str">
-        <f ca="1">IF(A26 = "TBA", "TBA", IF(A26 - TODAY() &gt; 0, A26 - TODAY(), "out now"))</f>
+        <f t="shared" ref="B26:B34" ca="1" si="7">IF(A26 = "TBA", "TBA", IF(A26 - TODAY() &gt; 0, A26 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>11</v>
@@ -1206,11 +1200,11 @@
         <v>45317</v>
       </c>
       <c r="B27" s="5" t="str">
-        <f ca="1">IF(A27 = "TBA", "TBA", IF(A27 - TODAY() &gt; 0, A27 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>out now</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>35</v>
@@ -1221,11 +1215,11 @@
         <v>45345</v>
       </c>
       <c r="B28" s="5">
-        <f ca="1">IF(A28 = "TBA", "TBA", IF(A28 - TODAY() &gt; 0, A28 - TODAY(), "out now"))</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>12</v>
@@ -1239,11 +1233,11 @@
         <v>45345</v>
       </c>
       <c r="B29" s="5">
-        <f ca="1">IF(A29 = "TBA", "TBA", IF(A29 - TODAY() &gt; 0, A29 - TODAY(), "out now"))</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>24</v>
@@ -1254,17 +1248,17 @@
         <v>45345</v>
       </c>
       <c r="B30" s="5">
-        <f ca="1">IF(A30 = "TBA", "TBA", IF(A30 - TODAY() &gt; 0, A30 - TODAY(), "out now"))</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" t="s">
         <v>95</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1272,14 +1266,14 @@
         <v>45352</v>
       </c>
       <c r="B31" s="5">
-        <f ca="1">IF(A31 = "TBA", "TBA", IF(A31 - TODAY() &gt; 0, A31 - TODAY(), "out now"))</f>
-        <v>11</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>10</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1287,11 +1281,11 @@
         <v>45352</v>
       </c>
       <c r="B32" s="5">
-        <f ca="1">IF(A32 = "TBA", "TBA", IF(A32 - TODAY() &gt; 0, A32 - TODAY(), "out now"))</f>
-        <v>11</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>10</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>12</v>
@@ -1302,11 +1296,11 @@
         <v>45373</v>
       </c>
       <c r="B33" s="5">
-        <f ca="1">IF(A33 = "TBA", "TBA", IF(A33 - TODAY() &gt; 0, A33 - TODAY(), "out now"))</f>
-        <v>32</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>31</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>13</v>
@@ -1317,11 +1311,11 @@
         <v>45387</v>
       </c>
       <c r="B34" s="5">
-        <f ca="1">IF(A34 = "TBA", "TBA", IF(A34 - TODAY() &gt; 0, A34 - TODAY(), "out now"))</f>
-        <v>46</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>12</v>
@@ -1646,7 +1640,7 @@
       </c>
       <c r="B17" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>42</v>
@@ -1664,7 +1658,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="5"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Add Temporal Forces ultra rares
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894AFF34-E14B-4CEA-B5A2-CAC84A90D245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388D33F5-A6D1-4521-9B70-82AC558946C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -297,9 +297,6 @@
     <t>Fall 2023 Collector Chest</t>
   </si>
   <si>
-    <t>ultra rares added, also check blister promos</t>
-  </si>
-  <si>
     <t>Paldea Friends Mini Tin 5-Pack</t>
   </si>
   <si>
@@ -343,6 +340,27 @@
   </si>
   <si>
     <t>Iono Premium Tournament Collection</t>
+  </si>
+  <si>
+    <t>Paradox Clash Tins</t>
+  </si>
+  <si>
+    <t>Twilight Masquerade</t>
+  </si>
+  <si>
+    <t>Armarouge ex Premium Collection</t>
+  </si>
+  <si>
+    <t>Grafaiai ex Box</t>
+  </si>
+  <si>
+    <t>Triple Whammy Tin</t>
+  </si>
+  <si>
+    <t>check blister promos</t>
+  </si>
+  <si>
+    <t>ultra rares added</t>
   </si>
 </sst>
 </file>
@@ -745,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1060,7 +1078,7 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1078,7 +1096,7 @@
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1105,13 +1123,13 @@
         <v>out now</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1159,7 +1177,7 @@
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1182,17 +1200,17 @@
         <v>45296</v>
       </c>
       <c r="B26" s="5" t="str">
-        <f t="shared" ref="B26:B34" ca="1" si="7">IF(A26 = "TBA", "TBA", IF(A26 - TODAY() &gt; 0, A26 - TODAY(), "out now"))</f>
+        <f t="shared" ref="B26:B33" ca="1" si="7">IF(A26 = "TBA", "TBA", IF(A26 - TODAY() &gt; 0, A26 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1204,7 +1222,7 @@
         <v>out now</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>35</v>
@@ -1214,30 +1232,30 @@
       <c r="A28" s="7">
         <v>45345</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>out now</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>45345</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>out now</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>24</v>
@@ -1247,78 +1265,156 @@
       <c r="A30" s="7">
         <v>45345</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>out now</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" t="s">
         <v>94</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E30" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>45352</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>10</v>
+        <v>out now</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>45352</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>10</v>
+        <v>out now</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="7">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
         <v>45373</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>31</v>
-      </c>
-      <c r="C33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>45383</v>
+      </c>
+      <c r="B34" s="5">
+        <f ca="1">IF(A34 = "TBA", "TBA", IF(A34 - TODAY() &gt; 0, A34 - TODAY(), "out now"))</f>
+        <v>11</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>45387</v>
+      </c>
+      <c r="B35" s="5">
+        <f ca="1">IF(A35 = "TBA", "TBA", IF(A35 - TODAY() &gt; 0, A35 - TODAY(), "out now"))</f>
+        <v>15</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D35" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>45387</v>
+      </c>
+      <c r="B36" s="5">
+        <f t="shared" ref="B36" ca="1" si="8">IF(A36 = "TBA", "TBA", IF(A36 - TODAY() &gt; 0, A36 - TODAY(), "out now"))</f>
+        <v>15</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>45401</v>
+      </c>
+      <c r="B37" s="5">
+        <f ca="1">IF(A37 = "TBA", "TBA", IF(A37 - TODAY() &gt; 0, A37 - TODAY(), "out now"))</f>
+        <v>29</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>45436</v>
+      </c>
+      <c r="B38" s="5">
+        <f t="shared" ref="B38" ca="1" si="9">IF(A38 = "TBA", "TBA", IF(A38 - TODAY() &gt; 0, A38 - TODAY(), "out now"))</f>
+        <v>64</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="7">
-        <v>45387</v>
-      </c>
-      <c r="B34" s="5">
-        <f t="shared" ca="1" si="7"/>
-        <v>45</v>
-      </c>
-      <c r="C34" s="5" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>45436</v>
+      </c>
+      <c r="B39" s="5">
+        <f ca="1">IF(A39 = "TBA", "TBA", IF(A39 - TODAY() &gt; 0, A39 - TODAY(), "out now"))</f>
+        <v>64</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>12</v>
+      <c r="D39" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1638,9 +1734,9 @@
       <c r="A17" s="7">
         <v>45359</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="5" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>17</v>
+        <v>out now</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>42</v>
@@ -1658,7 +1754,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="5"/>
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Add SVP ultra rares, update future cards
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388D33F5-A6D1-4521-9B70-82AC558946C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B160F190-75C6-4C97-BA34-29AB1DFAFE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
@@ -324,9 +324,6 @@
     <t>check holo</t>
   </si>
   <si>
-    <t>some cards from Pokémon TCG Classic</t>
-  </si>
-  <si>
     <t>2023 World Championships Decks</t>
   </si>
   <si>
@@ -361,6 +358,9 @@
   </si>
   <si>
     <t>ultra rares added</t>
+  </si>
+  <si>
+    <t>ultra rares added, cosmos (pixel only?)</t>
   </si>
 </sst>
 </file>
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,7 +1078,7 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1214,68 +1214,65 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
+      <c r="A27" s="8">
         <v>45317</v>
       </c>
-      <c r="B27" s="5" t="str">
+      <c r="B27" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>out now</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
+      <c r="A28" s="8">
         <v>45345</v>
       </c>
-      <c r="B28" s="5" t="str">
+      <c r="B28" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>out now</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="7">
+      <c r="A29" s="8">
         <v>45345</v>
       </c>
-      <c r="B29" s="5" t="str">
+      <c r="B29" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>out now</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="7">
+      <c r="A30" s="9">
         <v>45345</v>
       </c>
-      <c r="B30" s="5" t="str">
+      <c r="B30" s="3" t="str">
         <f t="shared" ca="1" si="7"/>
         <v>out now</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D30" s="3" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1288,25 +1285,28 @@
         <v>out now</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="5" t="s">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
+        <v>45352</v>
+      </c>
+      <c r="B32" s="2" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>out now</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="7">
-        <v>45352</v>
-      </c>
-      <c r="B32" s="5" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>out now</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1318,13 +1318,13 @@
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1336,7 +1336,7 @@
         <v>11</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>11</v>
@@ -1351,7 +1351,7 @@
         <v>15</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>12</v>
@@ -1366,7 +1366,7 @@
         <v>15</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>12</v>
@@ -1381,7 +1381,7 @@
         <v>29</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>12</v>
@@ -1396,7 +1396,7 @@
         <v>64</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>13</v>
@@ -1411,7 +1411,7 @@
         <v>64</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Add Stellar Crown ultra rares and some missing holos
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028654C9-BE81-40A3-86C5-CB41A012CE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B043A72A-2419-49BF-9ABA-20AD5F08309C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="3360" yWindow="2064" windowWidth="12648" windowHeight="8880" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="165">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -234,9 +234,6 @@
     <t>Venusaur &amp; Charizard &amp; Blastoise Special Deck Set ex</t>
   </si>
   <si>
-    <t>Fall 2023 Collector Chest</t>
-  </si>
-  <si>
     <t>Paldea Friends Mini Tin 5-Pack</t>
   </si>
   <si>
@@ -285,211 +282,256 @@
     <t>Triple Whammy Tin</t>
   </si>
   <si>
+    <t>Battle Academy 2024</t>
+  </si>
+  <si>
+    <t>Palafin ex Box</t>
+  </si>
+  <si>
+    <t>Night Wanderer</t>
+  </si>
+  <si>
+    <t>Mask of Change</t>
+  </si>
+  <si>
+    <t>Bloodmoon Ursaluna ex</t>
+  </si>
+  <si>
+    <t>Stellar Miracle</t>
+  </si>
+  <si>
+    <t>Paradise Dragona</t>
+  </si>
+  <si>
+    <t>Ogerpon Special Set</t>
+  </si>
+  <si>
+    <t>Starter Set Tera Type Stellar</t>
+  </si>
+  <si>
+    <t>Charizard &amp; Chien-Pao ex Battle Master Deck</t>
+  </si>
+  <si>
+    <t>ex Starter Decks: Generations</t>
+  </si>
+  <si>
+    <t>Supercharged Breaker</t>
+  </si>
+  <si>
+    <t>Stellar Terapagos ex</t>
+  </si>
+  <si>
+    <t>Stellar Pikachu ex</t>
+  </si>
+  <si>
+    <t>Ogerpon</t>
+  </si>
+  <si>
+    <t>Tera Charizard ex</t>
+  </si>
+  <si>
+    <t>Victini &amp; Miraidon ex Battle Decks</t>
+  </si>
+  <si>
+    <t>Palafin, Baxcalibur &amp; Garganacl Blister</t>
+  </si>
+  <si>
+    <t>Shrouded Fable</t>
+  </si>
+  <si>
+    <t>Terastal Festival</t>
+  </si>
+  <si>
+    <t>The Glory of Team Rocket</t>
+  </si>
+  <si>
+    <t>Main Set(?)</t>
+  </si>
+  <si>
+    <t>Paradox Destinies Tins</t>
+  </si>
+  <si>
+    <t>Trick or Trade BOOster Bundle 2024</t>
+  </si>
+  <si>
+    <t>Holiday Calendar 2024</t>
+  </si>
+  <si>
+    <t>Collector Chest (Back-to-School 2024)</t>
+  </si>
+  <si>
+    <t>Stellar Crown</t>
+  </si>
+  <si>
+    <t>Eeveelution Tera / Stellar ex's(?)</t>
+  </si>
+  <si>
+    <t>Battle Partners</t>
+  </si>
+  <si>
+    <t>Side Set(?)</t>
+  </si>
+  <si>
+    <t>Starter Set ex Steven &amp; Marnie</t>
+  </si>
+  <si>
+    <t>Koraidon ex, Miraidon ex, Gen 9</t>
+  </si>
+  <si>
+    <t>Lucario ex, Ampharos ex, Mimikyu ex</t>
+  </si>
+  <si>
+    <t>Meowscarada ex, Skeledirge ex, Quaquaval ex</t>
+  </si>
+  <si>
+    <t>Wo-Chien ex, Chien-Pao ex, Ting-Lu ex, Chi-Yu ex</t>
+  </si>
+  <si>
+    <t>Toedscruel ex, Pawmot ex, Houndstone ex</t>
+  </si>
+  <si>
+    <t>Tera Mewtwo ex, Tera Skeledirge ex</t>
+  </si>
+  <si>
+    <t>Roaring Moon ex, Iron Valiant ex</t>
+  </si>
+  <si>
+    <t>Venusaur ex, Charizard ex, Blastoise ex</t>
+  </si>
+  <si>
+    <t>Walking Wake ex, Iron Leaves ex</t>
+  </si>
+  <si>
+    <t>Koraidon ex, Miraidon ex</t>
+  </si>
+  <si>
+    <t>Meowscarada ex, Pikachu ex, Lucario ex, Greninja ex</t>
+  </si>
+  <si>
+    <t>4 Tera Ogerpon ex</t>
+  </si>
+  <si>
+    <t>Tera Charizard ex, Chien-Pao ex</t>
+  </si>
+  <si>
+    <t>Pecharunt ex, Okidogi ex, Munkidori ex, Fezandipiti ex</t>
+  </si>
+  <si>
+    <t>Stellar Sylveon ex, Stellar Ceruledge ex</t>
+  </si>
+  <si>
+    <t>9 Legendary ex's, 9 other ex's</t>
+  </si>
+  <si>
+    <t>Owner’s ex</t>
+  </si>
+  <si>
+    <t>Dark / Rocket's Pokémon ex(?)</t>
+  </si>
+  <si>
+    <t>Surging Sparks</t>
+  </si>
+  <si>
+    <t>Houndstone ex Box</t>
+  </si>
+  <si>
+    <t>Charizard ex Super-Premium Collection</t>
+  </si>
+  <si>
+    <t>Stellar Alolan Exeggutor ex, Latias ex</t>
+  </si>
+  <si>
+    <t>Prize Pack Series 5</t>
+  </si>
+  <si>
+    <t>Terapagos ex Ultra-Premium Collection</t>
+  </si>
+  <si>
+    <t>ultra rare promos + holo promos</t>
+  </si>
+  <si>
+    <t>are the holos actually ultra rares?</t>
+  </si>
+  <si>
+    <t>Steven’s Metagross ex, Marnie’s Grimmsnarl ex</t>
+  </si>
+  <si>
+    <t>Grand Adventure Collection</t>
+  </si>
+  <si>
+    <t>holo promos + exclusive jumbo</t>
+  </si>
+  <si>
+    <t>jumbo added</t>
+  </si>
+  <si>
+    <t>pixel cosmos + snowflake</t>
+  </si>
+  <si>
+    <t>Prize Pack Series 3</t>
+  </si>
+  <si>
+    <t>Prize Pack Series 4</t>
+  </si>
+  <si>
+    <t>holo is regular reverse</t>
+  </si>
+  <si>
+    <t>same as Classic</t>
+  </si>
+  <si>
+    <t>Espathra Two Pack Blister</t>
+  </si>
+  <si>
+    <t>Mc Donnalds 2024</t>
+  </si>
+  <si>
+    <t>Collector Chest Fall 2024</t>
+  </si>
+  <si>
+    <t>Collector Chest Fall 2023</t>
+  </si>
+  <si>
+    <t>Charizard ex League Battle Deck</t>
+  </si>
+  <si>
+    <t>check Charizard ex</t>
+  </si>
+  <si>
+    <t>Bloodmoon Ursaluna ex Box</t>
+  </si>
+  <si>
+    <t>Ogerpon ex Premium Collection</t>
+  </si>
+  <si>
+    <t>maybe has ultra rares?</t>
+  </si>
+  <si>
+    <t>Trainer’s Toolkit 2024</t>
+  </si>
+  <si>
+    <t>Lycanroc ex Box</t>
+  </si>
+  <si>
+    <t>ultra rare promo (metal)</t>
+  </si>
+  <si>
+    <t>Greninja ex Ultra-Premium Collection</t>
+  </si>
+  <si>
+    <t>description mentions Full Art</t>
+  </si>
+  <si>
     <t>ultra rares added</t>
   </si>
   <si>
-    <t>Battle Academy 2024</t>
-  </si>
-  <si>
-    <t>Palafin ex Box</t>
-  </si>
-  <si>
-    <t>Night Wanderer</t>
-  </si>
-  <si>
-    <t>Mask of Change</t>
-  </si>
-  <si>
-    <t>Bloodmoon Ursaluna ex</t>
-  </si>
-  <si>
-    <t>Stellar Miracle</t>
-  </si>
-  <si>
-    <t>Paradise Dragona</t>
-  </si>
-  <si>
-    <t>Ogerpon Special Set</t>
-  </si>
-  <si>
-    <t>Starter Set Tera Type Stellar</t>
-  </si>
-  <si>
-    <t>Charizard &amp; Chien-Pao ex Battle Master Deck</t>
-  </si>
-  <si>
-    <t>ex Starter Decks: Generations</t>
-  </si>
-  <si>
-    <t>Supercharged Breaker</t>
-  </si>
-  <si>
-    <t>Stellar Terapagos ex</t>
-  </si>
-  <si>
-    <t>Stellar Pikachu ex</t>
-  </si>
-  <si>
-    <t>Ogerpon</t>
-  </si>
-  <si>
-    <t>Tera Charizard ex</t>
-  </si>
-  <si>
-    <t>Victini &amp; Miraidon ex Battle Decks</t>
-  </si>
-  <si>
-    <t>Palafin, Baxcalibur &amp; Garganacl Blister</t>
-  </si>
-  <si>
-    <t>Shrouded Fable</t>
-  </si>
-  <si>
-    <t>Terastal Festival</t>
-  </si>
-  <si>
-    <t>The Glory of Team Rocket</t>
-  </si>
-  <si>
-    <t>Main Set(?)</t>
-  </si>
-  <si>
-    <t>Paradox Destinies Tins</t>
-  </si>
-  <si>
-    <t>Trick or Trade BOOster Bundle 2024</t>
-  </si>
-  <si>
-    <t>Holiday Calendar 2024</t>
-  </si>
-  <si>
-    <t>Collector Chest (Back-to-School 2024)</t>
-  </si>
-  <si>
-    <t>Stellar Crown</t>
-  </si>
-  <si>
-    <t>Eeveelution Tera / Stellar ex's(?)</t>
-  </si>
-  <si>
-    <t>Battle Partners</t>
-  </si>
-  <si>
-    <t>Side Set(?)</t>
-  </si>
-  <si>
-    <t>Starter Set ex Steven &amp; Marnie</t>
-  </si>
-  <si>
-    <t>Koraidon ex, Miraidon ex, Gen 9</t>
-  </si>
-  <si>
-    <t>Lucario ex, Ampharos ex, Mimikyu ex</t>
-  </si>
-  <si>
-    <t>Meowscarada ex, Skeledirge ex, Quaquaval ex</t>
-  </si>
-  <si>
-    <t>Wo-Chien ex, Chien-Pao ex, Ting-Lu ex, Chi-Yu ex</t>
-  </si>
-  <si>
-    <t>Toedscruel ex, Pawmot ex, Houndstone ex</t>
-  </si>
-  <si>
-    <t>Tera Mewtwo ex, Tera Skeledirge ex</t>
-  </si>
-  <si>
-    <t>Roaring Moon ex, Iron Valiant ex</t>
-  </si>
-  <si>
-    <t>Venusaur ex, Charizard ex, Blastoise ex</t>
-  </si>
-  <si>
-    <t>Walking Wake ex, Iron Leaves ex</t>
-  </si>
-  <si>
-    <t>Koraidon ex, Miraidon ex</t>
-  </si>
-  <si>
-    <t>Meowscarada ex, Pikachu ex, Lucario ex, Greninja ex</t>
-  </si>
-  <si>
-    <t>4 Tera Ogerpon ex</t>
-  </si>
-  <si>
-    <t>Tera Charizard ex, Chien-Pao ex</t>
-  </si>
-  <si>
-    <t>Pecharunt ex, Okidogi ex, Munkidori ex, Fezandipiti ex</t>
-  </si>
-  <si>
-    <t>Stellar Sylveon ex, Stellar Ceruledge ex</t>
-  </si>
-  <si>
-    <t>9 Legendary ex's, 9 other ex's</t>
-  </si>
-  <si>
-    <t>Owner’s ex</t>
-  </si>
-  <si>
-    <t>Dark / Rocket's Pokémon ex(?)</t>
-  </si>
-  <si>
-    <t>Surging Sparks</t>
-  </si>
-  <si>
-    <t>Houndstone ex Box</t>
-  </si>
-  <si>
-    <t>Charizard ex Super-Premium Collection</t>
-  </si>
-  <si>
-    <t>Stellar Alolan Exeggutor ex, Latias ex</t>
-  </si>
-  <si>
-    <t>Prize Pack Series 5</t>
-  </si>
-  <si>
-    <t>Terapagos ex Ultra-Premium Collection</t>
-  </si>
-  <si>
-    <t>ultra rare promos + holo promos</t>
-  </si>
-  <si>
-    <t>are the holos actually ultra rares?</t>
-  </si>
-  <si>
-    <t>Steven’s Metagross ex, Marnie’s Grimmsnarl ex</t>
-  </si>
-  <si>
-    <t>Grand Adventure Collection</t>
-  </si>
-  <si>
-    <t>holo promos + exclusive jumbo</t>
-  </si>
-  <si>
-    <t>jumbo added</t>
-  </si>
-  <si>
-    <t>pixel cosmos + snowflake</t>
-  </si>
-  <si>
-    <t>Prize Pack Series 3</t>
-  </si>
-  <si>
-    <t>Prize Pack Series 4</t>
-  </si>
-  <si>
-    <t>holo is regular reverse</t>
-  </si>
-  <si>
-    <t>same as Classic</t>
-  </si>
-  <si>
-    <t>Espathra Two Pack Blister</t>
-  </si>
-  <si>
-    <t>Mc Donnalds 2024</t>
+    <t>Decidueye ex Box</t>
+  </si>
+  <si>
+    <t>only revealed in Fr / Ger so far</t>
+  </si>
+  <si>
+    <t>Enhanced 2-Pack Blister</t>
   </si>
 </sst>
 </file>
@@ -901,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,7 +1039,7 @@
         <v>out now</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
@@ -1244,7 +1286,7 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1256,7 +1298,7 @@
         <v>out now</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>10</v>
@@ -1301,13 +1343,13 @@
         <v>out now</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1334,7 +1376,7 @@
         <v>out now</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>10</v>
@@ -1349,7 +1391,7 @@
         <v>out now</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>33</v>
@@ -1364,7 +1406,7 @@
         <v>out now</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>13</v>
@@ -1375,11 +1417,11 @@
         <v>45345</v>
       </c>
       <c r="B29" s="2" t="str">
-        <f ca="1">IF(A29 = "TBA", "TBA", IF(A29 - TODAY() &gt; 0, A29 - TODAY(), "out now"))</f>
+        <f t="shared" ref="B29:B36" ca="1" si="8">IF(A29 = "TBA", "TBA", IF(A29 - TODAY() &gt; 0, A29 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>11</v>
@@ -1390,11 +1432,11 @@
         <v>45345</v>
       </c>
       <c r="B30" s="2" t="str">
-        <f ca="1">IF(A30 = "TBA", "TBA", IF(A30 - TODAY() &gt; 0, A30 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>out now</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>23</v>
@@ -1405,15 +1447,15 @@
         <v>45345</v>
       </c>
       <c r="B31" s="3" t="str">
-        <f ca="1">IF(A31 = "TBA", "TBA", IF(A31 - TODAY() &gt; 0, A31 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>out now</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1421,110 +1463,107 @@
         <v>45352</v>
       </c>
       <c r="B32" s="4" t="str">
-        <f ca="1">IF(A32 = "TBA", "TBA", IF(A32 - TODAY() &gt; 0, A32 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>out now</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>45352</v>
       </c>
       <c r="B33" s="2" t="str">
-        <f ca="1">IF(A33 = "TBA", "TBA", IF(A33 - TODAY() &gt; 0, A33 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>out now</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="10">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
         <v>45373</v>
       </c>
-      <c r="B34" s="4" t="str">
-        <f ca="1">IF(A34 = "TBA", "TBA", IF(A34 - TODAY() &gt; 0, A34 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="B34" s="2" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>out now</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E34" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>45383</v>
       </c>
       <c r="B35" s="2" t="str">
-        <f ca="1">IF(A35 = "TBA", "TBA", IF(A35 - TODAY() &gt; 0, A35 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>out now</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>45387</v>
       </c>
       <c r="B36" s="2" t="str">
-        <f ca="1">IF(A36 = "TBA", "TBA", IF(A36 - TODAY() &gt; 0, A36 - TODAY(), "out now"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>out now</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>45387</v>
       </c>
       <c r="B37" s="2" t="str">
-        <f t="shared" ref="B37:B38" ca="1" si="8">IF(A37 = "TBA", "TBA", IF(A37 - TODAY() &gt; 0, A37 - TODAY(), "out now"))</f>
+        <f t="shared" ref="B37:B38" ca="1" si="9">IF(A37 = "TBA", "TBA", IF(A37 - TODAY() &gt; 0, A37 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>45393</v>
       </c>
       <c r="B38" s="2" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="9"/>
         <v>out now</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>45401</v>
       </c>
@@ -1533,148 +1572,142 @@
         <v>out now</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="10">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
         <v>45436</v>
       </c>
-      <c r="B40" s="4" t="str">
-        <f t="shared" ref="B40" ca="1" si="9">IF(A40 = "TBA", "TBA", IF(A40 - TODAY() &gt; 0, A40 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="B40" s="2" t="str">
+        <f t="shared" ref="B40" ca="1" si="10">IF(A40 = "TBA", "TBA", IF(A40 - TODAY() &gt; 0, A40 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>45436</v>
       </c>
       <c r="B41" s="2" t="str">
-        <f t="shared" ref="B41:B47" ca="1" si="10">IF(A41 = "TBA", "TBA", IF(A41 - TODAY() &gt; 0, A41 - TODAY(), "out now"))</f>
+        <f t="shared" ref="B41:B47" ca="1" si="11">IF(A41 = "TBA", "TBA", IF(A41 - TODAY() &gt; 0, A41 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>45464</v>
       </c>
       <c r="B42" s="2" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>out now</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>45464</v>
       </c>
       <c r="B43" s="2" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>out now</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="8">
         <v>45478</v>
       </c>
       <c r="B44" s="2" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>out now</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <v>45485</v>
       </c>
       <c r="B45" s="2" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>out now</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="10">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="8">
         <v>45506</v>
       </c>
-      <c r="B46" s="4" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>out now</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="B46" s="2" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>out now</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E46" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>45506</v>
       </c>
       <c r="B47" s="2" t="str">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="11"/>
         <v>out now</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
         <v>45518</v>
       </c>
       <c r="B48" s="2" t="str">
-        <f t="shared" ref="B48:B53" ca="1" si="11">IF(A48 = "TBA", "TBA", IF(A48 - TODAY() &gt; 0, A48 - TODAY(), "out now"))</f>
+        <f t="shared" ref="B48:B50" ca="1" si="12">IF(A48 = "TBA", "TBA", IF(A48 - TODAY() &gt; 0, A48 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>13</v>
@@ -1685,155 +1718,306 @@
         <v>45527</v>
       </c>
       <c r="B49" s="4" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>out now</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="7">
+      <c r="A50" s="10">
         <v>45534</v>
       </c>
-      <c r="B50" s="5">
-        <f t="shared" ca="1" si="11"/>
-        <v>7</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" s="5" t="s">
+      <c r="B50" s="4" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v>out now</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="7">
+      <c r="A51" s="10">
+        <v>45535</v>
+      </c>
+      <c r="B51" s="4" t="str">
+        <f t="shared" ref="B51" ca="1" si="13">IF(A51 = "TBA", "TBA", IF(A51 - TODAY() &gt; 0, A51 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="8">
         <v>45541</v>
       </c>
-      <c r="B51" s="5">
-        <f t="shared" ca="1" si="11"/>
-        <v>14</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D51" s="5" t="s">
+      <c r="B52" s="2" t="str">
+        <f ca="1">IF(A52 = "TBA", "TBA", IF(A52 - TODAY() &gt; 0, A52 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="7">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="10">
         <v>45548</v>
       </c>
-      <c r="B52" s="5">
-        <f t="shared" ca="1" si="11"/>
-        <v>21</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D52" s="5" t="s">
+      <c r="B53" s="4" t="str">
+        <f ca="1">IF(A53 = "TBA", "TBA", IF(A53 - TODAY() &gt; 0, A53 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="7">
-        <v>45569</v>
-      </c>
-      <c r="B53" s="5">
-        <f t="shared" ca="1" si="11"/>
-        <v>42</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>11</v>
+      <c r="E53" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
-        <v>45569</v>
+        <v>45585</v>
       </c>
       <c r="B54" s="5">
-        <f t="shared" ref="B54:B55" ca="1" si="12">IF(A54 = "TBA", "TBA", IF(A54 - TODAY() &gt; 0, A54 - TODAY(), "out now"))</f>
-        <v>42</v>
+        <f ca="1">IF(A54 = "TBA", "TBA", IF(A54 - TODAY() &gt; 0, A54 - TODAY(), "out now"))</f>
+        <v>36</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="E54" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
-        <v>45597</v>
+        <v>45569</v>
       </c>
       <c r="B55" s="5">
-        <f t="shared" ca="1" si="12"/>
-        <v>70</v>
+        <f ca="1">IF(A55 = "TBA", "TBA", IF(A55 - TODAY() &gt; 0, A55 - TODAY(), "out now"))</f>
+        <v>20</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E55" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
-        <v>45604</v>
+        <v>45569</v>
       </c>
       <c r="B56" s="5">
-        <f ca="1">IF(A56 = "TBA", "TBA", IF(A56 - TODAY() &gt; 0, A56 - TODAY(), "out now"))</f>
-        <v>77</v>
+        <f t="shared" ref="B56:B57" ca="1" si="14">IF(A56 = "TBA", "TBA", IF(A56 - TODAY() &gt; 0, A56 - TODAY(), "out now"))</f>
+        <v>20</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>132</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
-        <v>45604</v>
+        <v>45583</v>
       </c>
       <c r="B57" s="5">
-        <f ca="1">IF(A57 = "TBA", "TBA", IF(A57 - TODAY() &gt; 0, A57 - TODAY(), "out now"))</f>
-        <v>77</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>34</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E57" t="s">
-        <v>143</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
-        <v>45657</v>
+        <v>45597</v>
       </c>
       <c r="B58" s="5">
         <f ca="1">IF(A58 = "TBA", "TBA", IF(A58 - TODAY() &gt; 0, A58 - TODAY(), "out now"))</f>
+        <v>48</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E58" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="7">
+        <v>45597</v>
+      </c>
+      <c r="B59" s="5">
+        <f ca="1">IF(A59 = "TBA", "TBA", IF(A59 - TODAY() &gt; 0, A59 - TODAY(), "out now"))</f>
+        <v>48</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E59" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="7">
+        <v>45604</v>
+      </c>
+      <c r="B60" s="5">
+        <f t="shared" ref="B60:B67" ca="1" si="15">IF(A60 = "TBA", "TBA", IF(A60 - TODAY() &gt; 0, A60 - TODAY(), "out now"))</f>
+        <v>55</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D58" s="5" t="s">
+      <c r="D60" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="7">
+        <v>45604</v>
+      </c>
+      <c r="B61" s="5">
+        <f t="shared" ca="1" si="15"/>
+        <v>55</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E61" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="7">
+        <v>45611</v>
+      </c>
+      <c r="B62" s="5">
+        <f t="shared" ca="1" si="15"/>
+        <v>62</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="9">
+        <v>45611</v>
+      </c>
+      <c r="B63" s="3">
+        <f t="shared" ca="1" si="15"/>
+        <v>62</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63" s="3"/>
+      <c r="E63" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="7">
+        <v>45611</v>
+      </c>
+      <c r="B64" s="5">
+        <f t="shared" ca="1" si="15"/>
+        <v>62</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="7">
+        <v>45611</v>
+      </c>
+      <c r="B65" s="5">
+        <f t="shared" ca="1" si="15"/>
+        <v>62</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="7">
+        <v>45657</v>
+      </c>
+      <c r="B66" s="5">
+        <f t="shared" ca="1" si="15"/>
+        <v>108</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="7">
+        <v>45657</v>
+      </c>
+      <c r="B67" s="5">
+        <f t="shared" ca="1" si="15"/>
+        <v>108</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1876,7 +2060,7 @@
         <v>42</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1894,7 +2078,7 @@
         <v>43</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1912,7 +2096,7 @@
         <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1948,7 +2132,7 @@
         <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1966,7 +2150,7 @@
         <v>43</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2020,7 +2204,7 @@
         <v>42</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -2056,7 +2240,7 @@
         <v>43</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2074,7 +2258,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2092,7 +2276,7 @@
         <v>43</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2128,7 +2312,7 @@
         <v>42</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2146,7 +2330,7 @@
         <v>43</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -2164,7 +2348,7 @@
         <v>43</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -2182,7 +2366,7 @@
         <v>49</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -2194,13 +2378,13 @@
         <v>out now</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -2212,13 +2396,13 @@
         <v>out now</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2230,13 +2414,13 @@
         <v>out now</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2248,13 +2432,13 @@
         <v>out now</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2266,49 +2450,49 @@
         <v>out now</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>45534</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="5" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>out now</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>45548</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>21</v>
+        <v>out now</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -2317,16 +2501,16 @@
       </c>
       <c r="B26" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -2335,16 +2519,16 @@
       </c>
       <c r="B27" s="5">
         <f t="shared" ca="1" si="6"/>
+        <v>69</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2353,16 +2537,16 @@
       </c>
       <c r="B28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -2371,16 +2555,16 @@
       </c>
       <c r="B29" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -2389,16 +2573,16 @@
       </c>
       <c r="B30" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -2407,16 +2591,16 @@
       </c>
       <c r="B31" s="4">
         <f ca="1">IF(A31 = "TBA", "TBA", IF(A31 - TODAY() &gt; 0, A31 - TODAY(), "out now"))</f>
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 26/9/2024, add Genetix Apex pocket cards
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B043A72A-2419-49BF-9ABA-20AD5F08309C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7D4DF2-DD54-4E6C-8514-B3B0DDBA46B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2064" windowWidth="12648" windowHeight="8880" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="12648" windowHeight="8880" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1793,11 +1793,11 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
-        <v>45585</v>
+        <v>45555</v>
       </c>
       <c r="B54" s="5">
         <f ca="1">IF(A54 = "TBA", "TBA", IF(A54 - TODAY() &gt; 0, A54 - TODAY(), "out now"))</f>
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>162</v>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="B55" s="5">
         <f ca="1">IF(A55 = "TBA", "TBA", IF(A55 - TODAY() &gt; 0, A55 - TODAY(), "out now"))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>131</v>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="B56" s="5">
         <f t="shared" ref="B56:B57" ca="1" si="14">IF(A56 = "TBA", "TBA", IF(A56 - TODAY() &gt; 0, A56 - TODAY(), "out now"))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>132</v>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="B57" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>156</v>
@@ -1860,7 +1860,7 @@
       </c>
       <c r="B58" s="5">
         <f ca="1">IF(A58 = "TBA", "TBA", IF(A58 - TODAY() &gt; 0, A58 - TODAY(), "out now"))</f>
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>135</v>
@@ -1878,7 +1878,7 @@
       </c>
       <c r="B59" s="5">
         <f ca="1">IF(A59 = "TBA", "TBA", IF(A59 - TODAY() &gt; 0, A59 - TODAY(), "out now"))</f>
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>159</v>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="B60" s="5">
         <f t="shared" ref="B60:B67" ca="1" si="15">IF(A60 = "TBA", "TBA", IF(A60 - TODAY() &gt; 0, A60 - TODAY(), "out now"))</f>
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>130</v>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="B61" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>139</v>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="B62" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>149</v>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="B63" s="3">
         <f t="shared" ca="1" si="15"/>
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>151</v>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="B64" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>153</v>
@@ -1978,7 +1978,7 @@
       </c>
       <c r="B65" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>154</v>
@@ -1993,7 +1993,7 @@
       </c>
       <c r="B66" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>148</v>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="B67" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>164</v>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="B26" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>92</v>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="B27" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>91</v>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="B28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>100</v>
@@ -2555,7 +2555,7 @@
       </c>
       <c r="B29" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>109</v>
@@ -2573,7 +2573,7 @@
       </c>
       <c r="B30" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>111</v>
@@ -2591,7 +2591,7 @@
       </c>
       <c r="B31" s="4">
         <f ca="1">IF(A31 = "TBA", "TBA", IF(A31 - TODAY() &gt; 0, A31 - TODAY(), "out now"))</f>
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Add Pocket holo promos
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB3D8ED-916D-4AEB-8407-F95AA27378A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A746DFE-5920-447D-9659-FBA47736E0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10392" yWindow="3312" windowWidth="12648" windowHeight="8880" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="12648" windowHeight="8880" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="171">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -535,6 +535,21 @@
   </si>
   <si>
     <t>Legendary Warriors Premium Collection</t>
+  </si>
+  <si>
+    <t>4 cosmos store promos</t>
+  </si>
+  <si>
+    <t>151 5-pack Mini Tins Bundle</t>
+  </si>
+  <si>
+    <t>Meddling Sparks Premium Collection</t>
+  </si>
+  <si>
+    <t>check Scizor and Luxray</t>
+  </si>
+  <si>
+    <t>holo promos(?)</t>
   </si>
 </sst>
 </file>
@@ -946,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C56" sqref="C55:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1846,9 +1861,9 @@
       <c r="A57" s="7">
         <v>45576</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B57" s="5" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>1</v>
+        <v>out now</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>165</v>
@@ -1861,9 +1876,9 @@
       <c r="A58" s="7">
         <v>45583</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="5" t="str">
         <f ca="1">IF(A58 = "TBA", "TBA", IF(A58 - TODAY() &gt; 0, A58 - TODAY(), "out now"))</f>
-        <v>8</v>
+        <v>out now</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>155</v>
@@ -1874,105 +1889,107 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
-        <v>45597</v>
-      </c>
-      <c r="B59" s="5">
+        <v>45586</v>
+      </c>
+      <c r="B59" s="5" t="str">
         <f ca="1">IF(A59 = "TBA", "TBA", IF(A59 - TODAY() &gt; 0, A59 - TODAY(), "out now"))</f>
-        <v>22</v>
+        <v>out now</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E59" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
-        <v>45597</v>
-      </c>
-      <c r="B60" s="5">
+        <v>45596</v>
+      </c>
+      <c r="B60" s="5" t="str">
         <f ca="1">IF(A60 = "TBA", "TBA", IF(A60 - TODAY() &gt; 0, A60 - TODAY(), "out now"))</f>
-        <v>22</v>
+        <v>out now</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="E60" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
-        <v>45604</v>
-      </c>
-      <c r="B61" s="5">
-        <f t="shared" ref="B61:B68" ca="1" si="15">IF(A61 = "TBA", "TBA", IF(A61 - TODAY() &gt; 0, A61 - TODAY(), "out now"))</f>
-        <v>29</v>
+        <v>45597</v>
+      </c>
+      <c r="B61" s="5" t="str">
+        <f ca="1">IF(A61 = "TBA", "TBA", IF(A61 - TODAY() &gt; 0, A61 - TODAY(), "out now"))</f>
+        <v>out now</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>12</v>
+        <v>135</v>
+      </c>
+      <c r="E61" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
-        <v>45604</v>
-      </c>
-      <c r="B62" s="5">
-        <f t="shared" ca="1" si="15"/>
-        <v>29</v>
+        <v>45597</v>
+      </c>
+      <c r="B62" s="5" t="str">
+        <f ca="1">IF(A62 = "TBA", "TBA", IF(A62 - TODAY() &gt; 0, A62 - TODAY(), "out now"))</f>
+        <v>out now</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="E62" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
+        <v>45604</v>
+      </c>
+      <c r="B63" s="5" t="str">
+        <f t="shared" ref="B63:B70" ca="1" si="15">IF(A63 = "TBA", "TBA", IF(A63 - TODAY() &gt; 0, A63 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="7">
         <v>45611</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B64" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>36</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="9">
-        <v>45611</v>
-      </c>
-      <c r="B64" s="3">
-        <f t="shared" ca="1" si="15"/>
-        <v>36</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D64" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="E64" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1981,60 +1998,94 @@
       </c>
       <c r="B65" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>135</v>
+        <v>10</v>
+      </c>
+      <c r="E65" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="7">
+      <c r="A66" s="9">
         <v>45611</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B66" s="3">
         <f t="shared" ca="1" si="15"/>
-        <v>36</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>135</v>
+        <v>1</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="7">
-        <v>45657</v>
+        <v>45611</v>
       </c>
       <c r="B67" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="7">
-        <v>45657</v>
+        <v>45611</v>
       </c>
       <c r="B68" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="C68" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="7">
+        <v>45657</v>
+      </c>
+      <c r="B69" s="5">
+        <f t="shared" ca="1" si="15"/>
+        <v>47</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="7">
+        <v>45657</v>
+      </c>
+      <c r="B70" s="5">
+        <f t="shared" ca="1" si="15"/>
+        <v>47</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D70" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E70" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2517,9 +2568,9 @@
       <c r="A26" s="11">
         <v>45583</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="12" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>out now</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>92</v>
@@ -2537,7 +2588,7 @@
       </c>
       <c r="B27" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>91</v>
@@ -2555,7 +2606,7 @@
       </c>
       <c r="B28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>100</v>
@@ -2573,7 +2624,7 @@
       </c>
       <c r="B29" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>109</v>
@@ -2591,7 +2642,7 @@
       </c>
       <c r="B30" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>111</v>
@@ -2609,7 +2660,7 @@
       </c>
       <c r="B31" s="4">
         <f ca="1">IF(A31 = "TBA", "TBA", IF(A31 - TODAY() &gt; 0, A31 - TODAY(), "out now"))</f>
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Add Surging Sparks + promo Ultra Rares
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A746DFE-5920-447D-9659-FBA47736E0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FC646B-56F8-49B6-BEE6-331F21DE3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="12648" windowHeight="8880" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="169">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -447,9 +447,6 @@
     <t>ultra rare promos + holo promos</t>
   </si>
   <si>
-    <t>are the holos actually ultra rares?</t>
-  </si>
-  <si>
     <t>Steven’s Metagross ex, Marnie’s Grimmsnarl ex</t>
   </si>
   <si>
@@ -501,9 +498,6 @@
     <t>Ogerpon ex Premium Collection</t>
   </si>
   <si>
-    <t>maybe has ultra rares?</t>
-  </si>
-  <si>
     <t>Trainer’s Toolkit 2024</t>
   </si>
   <si>
@@ -516,9 +510,6 @@
     <t>Greninja ex Ultra-Premium Collection</t>
   </si>
   <si>
-    <t>description mentions Full Art</t>
-  </si>
-  <si>
     <t>ultra rares added</t>
   </si>
   <si>
@@ -537,9 +528,6 @@
     <t>Legendary Warriors Premium Collection</t>
   </si>
   <si>
-    <t>4 cosmos store promos</t>
-  </si>
-  <si>
     <t>151 5-pack Mini Tins Bundle</t>
   </si>
   <si>
@@ -550,6 +538,12 @@
   </si>
   <si>
     <t>holo promos(?)</t>
+  </si>
+  <si>
+    <t>all 3 are pixel cosmos</t>
+  </si>
+  <si>
+    <t>ultra rares added, 4 store promos - check holo</t>
   </si>
 </sst>
 </file>
@@ -963,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C56" sqref="C55:C56"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,7 +1051,7 @@
         <v>out now</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
@@ -1304,7 +1298,7 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1361,13 +1355,13 @@
         <v>out now</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1424,7 +1418,7 @@
         <v>out now</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>13</v>
@@ -1473,7 +1467,7 @@
       </c>
       <c r="D31" s="3"/>
       <c r="E31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1710,7 +1704,7 @@
         <v>out now</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>10</v>
@@ -1770,7 +1764,7 @@
         <v>out now</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>10</v>
@@ -1806,7 +1800,7 @@
         <v>12</v>
       </c>
       <c r="E53" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1818,196 +1812,199 @@
         <v>out now</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E54" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="10">
+        <v>45569</v>
+      </c>
+      <c r="B55" s="4" t="str">
+        <f ca="1">IF(A55 = "TBA", "TBA", IF(A55 - TODAY() &gt; 0, A55 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="10">
+        <v>45569</v>
+      </c>
+      <c r="B56" s="4" t="str">
+        <f t="shared" ref="B56:B57" ca="1" si="14">IF(A56 = "TBA", "TBA", IF(A56 - TODAY() &gt; 0, A56 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="10">
+        <v>45576</v>
+      </c>
+      <c r="B57" s="4" t="str">
+        <f t="shared" ca="1" si="14"/>
+        <v>out now</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="7">
-        <v>45569</v>
-      </c>
-      <c r="B55" s="5" t="str">
-        <f ca="1">IF(A55 = "TBA", "TBA", IF(A55 - TODAY() &gt; 0, A55 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="7">
-        <v>45569</v>
-      </c>
-      <c r="B56" s="5" t="str">
-        <f t="shared" ref="B56:B57" ca="1" si="14">IF(A56 = "TBA", "TBA", IF(A56 - TODAY() &gt; 0, A56 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="7">
-        <v>45576</v>
-      </c>
-      <c r="B57" s="5" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v>out now</v>
-      </c>
-      <c r="C57" s="5" t="s">
+      <c r="D57" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="8">
+        <v>45583</v>
+      </c>
+      <c r="B58" s="2" t="str">
+        <f ca="1">IF(A58 = "TBA", "TBA", IF(A58 - TODAY() &gt; 0, A58 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="10">
+        <v>45586</v>
+      </c>
+      <c r="B59" s="4" t="str">
+        <f ca="1">IF(A59 = "TBA", "TBA", IF(A59 - TODAY() &gt; 0, A59 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="10">
+        <v>45596</v>
+      </c>
+      <c r="B60" s="4" t="str">
+        <f ca="1">IF(A60 = "TBA", "TBA", IF(A60 - TODAY() &gt; 0, A60 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E60" t="s">
         <v>165</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="7">
-        <v>45583</v>
-      </c>
-      <c r="B58" s="5" t="str">
-        <f ca="1">IF(A58 = "TBA", "TBA", IF(A58 - TODAY() &gt; 0, A58 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C58" s="5" t="s">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="10">
+        <v>45597</v>
+      </c>
+      <c r="B61" s="4" t="str">
+        <f ca="1">IF(A61 = "TBA", "TBA", IF(A61 - TODAY() &gt; 0, A61 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E61" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="8">
+        <v>45597</v>
+      </c>
+      <c r="B62" s="2" t="str">
+        <f ca="1">IF(A62 = "TBA", "TBA", IF(A62 - TODAY() &gt; 0, A62 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="7">
-        <v>45586</v>
-      </c>
-      <c r="B59" s="5" t="str">
-        <f ca="1">IF(A59 = "TBA", "TBA", IF(A59 - TODAY() &gt; 0, A59 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="7">
-        <v>45596</v>
-      </c>
-      <c r="B60" s="5" t="str">
-        <f ca="1">IF(A60 = "TBA", "TBA", IF(A60 - TODAY() &gt; 0, A60 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C60" s="5" t="s">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="10">
+        <v>45604</v>
+      </c>
+      <c r="B63" s="4" t="str">
+        <f t="shared" ref="B63:B70" ca="1" si="15">IF(A63 = "TBA", "TBA", IF(A63 - TODAY() &gt; 0, A63 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" t="s">
         <v>168</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="E60" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="7">
-        <v>45597</v>
-      </c>
-      <c r="B61" s="5" t="str">
-        <f ca="1">IF(A61 = "TBA", "TBA", IF(A61 - TODAY() &gt; 0, A61 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E61" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="7">
-        <v>45597</v>
-      </c>
-      <c r="B62" s="5" t="str">
-        <f ca="1">IF(A62 = "TBA", "TBA", IF(A62 - TODAY() &gt; 0, A62 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E62" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="7">
-        <v>45604</v>
-      </c>
-      <c r="B63" s="5" t="str">
-        <f t="shared" ref="B63:B70" ca="1" si="15">IF(A63 = "TBA", "TBA", IF(A63 - TODAY() &gt; 0, A63 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" t="s">
-        <v>166</v>
-      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="7">
+      <c r="A64" s="10">
         <v>45611</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="4">
         <f t="shared" ca="1" si="15"/>
         <v>1</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="E64" t="s">
         <v>139</v>
       </c>
-      <c r="E64" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="7">
+      <c r="A65" s="10">
         <v>45611</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="4">
         <f t="shared" ca="1" si="15"/>
         <v>1</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D65" s="5" t="s">
+      <c r="C65" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E65" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -2019,53 +2016,59 @@
         <v>1</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="7">
+      <c r="A67" s="10">
         <v>45611</v>
       </c>
-      <c r="B67" s="5">
+      <c r="B67" s="4">
         <f t="shared" ca="1" si="15"/>
         <v>1</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D67" s="5" t="s">
+      <c r="C67" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="E67" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="7">
+      <c r="A68" s="10">
         <v>45611</v>
       </c>
-      <c r="B68" s="5">
+      <c r="B68" s="4">
         <f t="shared" ca="1" si="15"/>
         <v>1</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D68" s="5" t="s">
+      <c r="C68" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D68" s="4" t="s">
         <v>135</v>
+      </c>
+      <c r="E68" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="7">
-        <v>45657</v>
+        <v>45630</v>
       </c>
       <c r="B69" s="5">
         <f t="shared" ca="1" si="15"/>
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>13</v>
@@ -2080,13 +2083,13 @@
         <v>47</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E70" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2597,7 +2600,7 @@
         <v>43</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2651,7 +2654,7 @@
         <v>43</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add Stellar Crown & Surging Sparks holo promos
</commit_message>
<xml_diff>
--- a/ReleaseTracker.xlsx
+++ b/ReleaseTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PHP\TCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FC646B-56F8-49B6-BEE6-331F21DE3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EC3ADA-DCE0-4F6D-8D8E-CB924FA8A1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="12648" windowHeight="8880" xr2:uid="{00BE8BFB-92E2-4A02-81B3-FAEA1550503C}"/>
   </bookViews>
   <sheets>
     <sheet name="ReleaseTracker" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="190">
   <si>
     <t>Obsidian Flames</t>
   </si>
@@ -489,9 +489,6 @@
     <t>Charizard ex League Battle Deck</t>
   </si>
   <si>
-    <t>check Charizard ex</t>
-  </si>
-  <si>
     <t>Bloodmoon Ursaluna ex Box</t>
   </si>
   <si>
@@ -516,9 +513,6 @@
     <t>Decidueye ex Box</t>
   </si>
   <si>
-    <t>only revealed in Fr / Ger so far</t>
-  </si>
-  <si>
     <t>Enhanced 2-Pack Blister</t>
   </si>
   <si>
@@ -543,7 +537,76 @@
     <t>all 3 are pixel cosmos</t>
   </si>
   <si>
-    <t>ultra rares added, 4 store promos - check holo</t>
+    <t>Paldean Fates 5-pack Mini Tins Bundle</t>
+  </si>
+  <si>
+    <t>reverse pixel cosmos</t>
+  </si>
+  <si>
+    <t>English confirmed, 3 pixel cosmos</t>
+  </si>
+  <si>
+    <t>English revealed by Intertoys &amp; Ebay</t>
+  </si>
+  <si>
+    <t>Prismatic Evolutions</t>
+  </si>
+  <si>
+    <t>Prismatic Evolutions - ETB</t>
+  </si>
+  <si>
+    <t>Prismatic Evolutions - Binder Collection</t>
+  </si>
+  <si>
+    <t>Prismatic Evolutions - Poster Collection</t>
+  </si>
+  <si>
+    <t>Prismatic Evolutions - Tech Sticker Collections (3)</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Tyranitar ex / Tsareena ex Premium Collections (2)</t>
+  </si>
+  <si>
+    <t>Prismatic Evolutions - Surprise Box</t>
+  </si>
+  <si>
+    <t>Prismatic Evolutions - 2-Pack Blister</t>
+  </si>
+  <si>
+    <t>Prismatic Evolutions - Accessory Pouch Collection</t>
+  </si>
+  <si>
+    <t>Prismatic Evolutions - Super-Premium Collection</t>
+  </si>
+  <si>
+    <t>Prismatic Evolutions - Premium Figure Collection</t>
+  </si>
+  <si>
+    <t>pixel cosmos</t>
+  </si>
+  <si>
+    <t>Tera Team Premium Collection</t>
+  </si>
+  <si>
+    <t>Tera Brawlers Premium Collection</t>
+  </si>
+  <si>
+    <t>Koraidon ex &amp; Miraidon ex Deluxe Battle Decks</t>
+  </si>
+  <si>
+    <t>Dark Powers ex Special Collection</t>
+  </si>
+  <si>
+    <t>Paradox Fury Premium Collection</t>
+  </si>
+  <si>
+    <t>Paradox Wisdom Premium Collection</t>
+  </si>
+  <si>
+    <t>promos and ultra rares added, 4 store promos - check holo</t>
   </si>
 </sst>
 </file>
@@ -626,7 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -640,6 +703,10 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -955,16 +1022,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C325CCEF-95C8-46A5-9777-4D9562BD7F1D}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="73.5546875" bestFit="1" customWidth="1"/>
@@ -1715,7 +1782,7 @@
         <v>45518</v>
       </c>
       <c r="B48" s="2" t="str">
-        <f t="shared" ref="B48:B50" ca="1" si="12">IF(A48 = "TBA", "TBA", IF(A48 - TODAY() &gt; 0, A48 - TODAY(), "out now"))</f>
+        <f t="shared" ref="B48:B49" ca="1" si="12">IF(A48 = "TBA", "TBA", IF(A48 - TODAY() &gt; 0, A48 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -1726,279 +1793,261 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="10">
-        <v>45527</v>
-      </c>
-      <c r="B49" s="4" t="str">
+      <c r="A49" s="9">
+        <v>45520</v>
+      </c>
+      <c r="B49" s="3" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>out now</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="C49" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="10">
+        <v>45527</v>
+      </c>
+      <c r="B50" s="4" t="str">
+        <f ca="1">IF(A50 = "TBA", "TBA", IF(A50 - TODAY() &gt; 0, A50 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="9">
+        <v>45527</v>
+      </c>
+      <c r="B51" s="3" t="str">
+        <f ca="1">IF(A51 = "TBA", "TBA", IF(A51 - TODAY() &gt; 0, A51 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="10">
         <v>45534</v>
       </c>
-      <c r="B50" s="4" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>out now</v>
-      </c>
-      <c r="C50" s="4" t="s">
+      <c r="B52" s="4" t="str">
+        <f ca="1">IF(A52 = "TBA", "TBA", IF(A52 - TODAY() &gt; 0, A52 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="10">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="9">
+        <v>45534</v>
+      </c>
+      <c r="B53" s="3" t="str">
+        <f ca="1">IF(A53 = "TBA", "TBA", IF(A53 - TODAY() &gt; 0, A53 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="10">
         <v>45535</v>
       </c>
-      <c r="B51" s="4" t="str">
-        <f t="shared" ref="B51" ca="1" si="13">IF(A51 = "TBA", "TBA", IF(A51 - TODAY() &gt; 0, A51 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D51" s="4" t="s">
+      <c r="B54" s="4" t="str">
+        <f t="shared" ref="B54" ca="1" si="13">IF(A54 = "TBA", "TBA", IF(A54 - TODAY() &gt; 0, A54 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="8">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="8">
         <v>45541</v>
       </c>
-      <c r="B52" s="2" t="str">
-        <f ca="1">IF(A52 = "TBA", "TBA", IF(A52 - TODAY() &gt; 0, A52 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="B55" s="2" t="str">
+        <f ca="1">IF(A55 = "TBA", "TBA", IF(A55 - TODAY() &gt; 0, A55 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="10">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="9">
+        <v>45541</v>
+      </c>
+      <c r="B56" s="3" t="str">
+        <f ca="1">IF(A56 = "TBA", "TBA", IF(A56 - TODAY() &gt; 0, A56 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="8">
         <v>45548</v>
       </c>
-      <c r="B53" s="4" t="str">
-        <f ca="1">IF(A53 = "TBA", "TBA", IF(A53 - TODAY() &gt; 0, A53 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C53" s="4" t="s">
+      <c r="B57" s="2" t="str">
+        <f ca="1">IF(A57 = "TBA", "TBA", IF(A57 - TODAY() &gt; 0, A57 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D57" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E57" s="14"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="10">
+        <v>45555</v>
+      </c>
+      <c r="B58" s="4" t="str">
+        <f ca="1">IF(A58 = "TBA", "TBA", IF(A58 - TODAY() &gt; 0, A58 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="7">
-        <v>45555</v>
-      </c>
-      <c r="B54" s="5" t="str">
-        <f ca="1">IF(A54 = "TBA", "TBA", IF(A54 - TODAY() &gt; 0, A54 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D54" s="5" t="s">
+      <c r="D58" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E54" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="10">
-        <v>45569</v>
-      </c>
-      <c r="B55" s="4" t="str">
-        <f ca="1">IF(A55 = "TBA", "TBA", IF(A55 - TODAY() &gt; 0, A55 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="10">
-        <v>45569</v>
-      </c>
-      <c r="B56" s="4" t="str">
-        <f t="shared" ref="B56:B57" ca="1" si="14">IF(A56 = "TBA", "TBA", IF(A56 - TODAY() &gt; 0, A56 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="10">
-        <v>45576</v>
-      </c>
-      <c r="B57" s="4" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v>out now</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="8">
-        <v>45583</v>
-      </c>
-      <c r="B58" s="2" t="str">
-        <f ca="1">IF(A58 = "TBA", "TBA", IF(A58 - TODAY() &gt; 0, A58 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>23</v>
+      <c r="E58" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="10">
-        <v>45586</v>
+        <v>45569</v>
       </c>
       <c r="B59" s="4" t="str">
         <f ca="1">IF(A59 = "TBA", "TBA", IF(A59 - TODAY() &gt; 0, A59 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="10">
-        <v>45596</v>
+        <v>45569</v>
       </c>
       <c r="B60" s="4" t="str">
-        <f ca="1">IF(A60 = "TBA", "TBA", IF(A60 - TODAY() &gt; 0, A60 - TODAY(), "out now"))</f>
+        <f t="shared" ref="B60:B61" ca="1" si="14">IF(A60 = "TBA", "TBA", IF(A60 - TODAY() &gt; 0, A60 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="E60" t="s">
-        <v>165</v>
+        <v>11</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="10">
-        <v>45597</v>
-      </c>
-      <c r="B61" s="4" t="str">
-        <f ca="1">IF(A61 = "TBA", "TBA", IF(A61 - TODAY() &gt; 0, A61 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E61" t="s">
-        <v>157</v>
-      </c>
+      <c r="A61" s="9">
+        <v>45569</v>
+      </c>
+      <c r="B61" s="3" t="str">
+        <f t="shared" ref="B61" ca="1" si="15">IF(A61 = "TBA", "TBA", IF(A61 - TODAY() &gt; 0, A61 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="8">
-        <v>45597</v>
-      </c>
-      <c r="B62" s="2" t="str">
+      <c r="A62" s="10">
+        <v>45576</v>
+      </c>
+      <c r="B62" s="4" t="str">
         <f ca="1">IF(A62 = "TBA", "TBA", IF(A62 - TODAY() &gt; 0, A62 - TODAY(), "out now"))</f>
         <v>out now</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>155</v>
+      <c r="C62" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="10">
-        <v>45604</v>
-      </c>
-      <c r="B63" s="4" t="str">
-        <f t="shared" ref="B63:B70" ca="1" si="15">IF(A63 = "TBA", "TBA", IF(A63 - TODAY() &gt; 0, A63 - TODAY(), "out now"))</f>
-        <v>out now</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" t="s">
-        <v>168</v>
+      <c r="A63" s="8">
+        <v>45583</v>
+      </c>
+      <c r="B63" s="2" t="str">
+        <f t="shared" ref="B63:B69" ca="1" si="16">IF(A63 = "TBA", "TBA", IF(A63 - TODAY() &gt; 0, A63 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="10">
-        <v>45611</v>
-      </c>
-      <c r="B64" s="4">
-        <f t="shared" ca="1" si="15"/>
-        <v>1</v>
+        <v>45586</v>
+      </c>
+      <c r="B64" s="4" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v>out now</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
       <c r="E64" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="10">
-        <v>45611</v>
-      </c>
-      <c r="B65" s="4">
-        <f t="shared" ca="1" si="15"/>
-        <v>1</v>
+        <v>45586</v>
+      </c>
+      <c r="B65" s="4" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v>out now</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>10</v>
@@ -2008,88 +2057,362 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="9">
-        <v>45611</v>
-      </c>
-      <c r="B66" s="3">
-        <f t="shared" ca="1" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D66" s="3"/>
+      <c r="A66" s="10">
+        <v>45586</v>
+      </c>
+      <c r="B66" s="4" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v>out now</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E66" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="10">
-        <v>45611</v>
-      </c>
-      <c r="B67" s="4">
-        <f t="shared" ca="1" si="15"/>
-        <v>1</v>
+        <v>45596</v>
+      </c>
+      <c r="B67" s="4" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v>out now</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="E67" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="10">
-        <v>45611</v>
-      </c>
-      <c r="B68" s="4">
-        <f t="shared" ca="1" si="15"/>
-        <v>1</v>
+        <v>45597</v>
+      </c>
+      <c r="B68" s="4" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v>out now</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E68" t="s">
-        <v>157</v>
+      <c r="E68" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="7">
+      <c r="A69" s="8">
+        <v>45597</v>
+      </c>
+      <c r="B69" s="2" t="str">
+        <f t="shared" ca="1" si="16"/>
+        <v>out now</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="10">
+        <v>45604</v>
+      </c>
+      <c r="B70" s="4" t="str">
+        <f t="shared" ref="B70:B75" ca="1" si="17">IF(A70 = "TBA", "TBA", IF(A70 - TODAY() &gt; 0, A70 - TODAY(), "out now"))</f>
+        <v>out now</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="10">
+        <v>45611</v>
+      </c>
+      <c r="B71" s="4" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v>out now</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="10">
+        <v>45611</v>
+      </c>
+      <c r="B72" s="4" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v>out now</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="9">
+        <v>45611</v>
+      </c>
+      <c r="B73" s="3" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v>out now</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="10">
+        <v>45611</v>
+      </c>
+      <c r="B74" s="4" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v>out now</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="10">
+        <v>45611</v>
+      </c>
+      <c r="B75" s="4" t="str">
+        <f t="shared" ca="1" si="17"/>
+        <v>out now</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="7">
+        <v>45625</v>
+      </c>
+      <c r="B76" s="5">
+        <f t="shared" ref="B76:B81" ca="1" si="18">IF(A76 = "TBA", "TBA", IF(A76 - TODAY() &gt; 0, A76 - TODAY(), "out now"))</f>
+        <v>13</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="7">
         <v>45630</v>
       </c>
-      <c r="B69" s="5">
-        <f t="shared" ca="1" si="15"/>
-        <v>20</v>
-      </c>
-      <c r="C69" s="5" t="s">
+      <c r="B77" s="5">
+        <f t="shared" ca="1" si="18"/>
+        <v>18</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D77" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="7">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="9">
         <v>45657</v>
       </c>
-      <c r="B70" s="5">
-        <f t="shared" ca="1" si="15"/>
-        <v>47</v>
-      </c>
-      <c r="C70" s="5" t="s">
+      <c r="B78" s="3">
+        <f t="shared" ca="1" si="18"/>
+        <v>45</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="7">
+        <v>45674</v>
+      </c>
+      <c r="B79" s="5">
+        <f t="shared" ca="1" si="18"/>
+        <v>62</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="7">
+        <v>45674</v>
+      </c>
+      <c r="B80" s="5">
+        <f t="shared" ca="1" si="18"/>
+        <v>62</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="9">
+        <v>45674</v>
+      </c>
+      <c r="B81" s="3">
+        <f t="shared" ca="1" si="18"/>
+        <v>62</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="7">
+        <v>45674</v>
+      </c>
+      <c r="B82" s="5">
+        <f t="shared" ref="B82" ca="1" si="19">IF(A82 = "TBA", "TBA", IF(A82 - TODAY() &gt; 0, A82 - TODAY(), "out now"))</f>
+        <v>62</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="7">
+        <v>45674</v>
+      </c>
+      <c r="B83" s="5">
+        <f t="shared" ref="B83:B84" ca="1" si="20">IF(A83 = "TBA", "TBA", IF(A83 - TODAY() &gt; 0, A83 - TODAY(), "out now"))</f>
+        <v>62</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="9">
+        <v>45695</v>
+      </c>
+      <c r="B84" s="3">
+        <f t="shared" ca="1" si="20"/>
+        <v>83</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D84" s="3"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="7">
+        <v>45709</v>
+      </c>
+      <c r="B85" s="5">
+        <f ca="1">IF(A85 = "TBA", "TBA", IF(A85 - TODAY() &gt; 0, A85 - TODAY(), "out now"))</f>
+        <v>97</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="9">
+        <v>45772</v>
+      </c>
+      <c r="B86" s="3">
+        <f ca="1">IF(A86 = "TBA", "TBA", IF(A86 - TODAY() &gt; 0, A86 - TODAY(), "out now"))</f>
         <v>160</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" t="s">
-        <v>159</v>
+      <c r="C86" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="7">
+        <v>45793</v>
+      </c>
+      <c r="B87" s="5">
+        <f ca="1">IF(A87 = "TBA", "TBA", IF(A87 - TODAY() &gt; 0, A87 - TODAY(), "out now"))</f>
+        <v>181</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="7">
+        <v>45926</v>
+      </c>
+      <c r="B88" s="5">
+        <f ca="1">IF(A88 = "TBA", "TBA", IF(A88 - TODAY() &gt; 0, A88 - TODAY(), "out now"))</f>
+        <v>314</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2591,7 +2914,7 @@
       </c>
       <c r="B27" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>91</v>
@@ -2600,7 +2923,7 @@
         <v>43</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2609,7 +2932,7 @@
       </c>
       <c r="B28" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>100</v>
@@ -2627,7 +2950,7 @@
       </c>
       <c r="B29" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>109</v>
@@ -2645,7 +2968,7 @@
       </c>
       <c r="B30" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>111</v>
@@ -2663,7 +2986,7 @@
       </c>
       <c r="B31" s="4">
         <f ca="1">IF(A31 = "TBA", "TBA", IF(A31 - TODAY() &gt; 0, A31 - TODAY(), "out now"))</f>
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>101</v>

</xml_diff>